<commit_message>
Had to reformat and expand on everything
Python is weird since it works by itself but not in uipath. rest works though
</commit_message>
<xml_diff>
--- a/RoboticEnterpriseFramework/Data/Output/Nation_Covid_MLData.xlsx
+++ b/RoboticEnterpriseFramework/Data/Output/Nation_Covid_MLData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mannj\Documents\UiPath\RoboticEnterpriseFramework\Data\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B10D2FB-9EBD-4286-92BA-E13C51396ACA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01125C1-3533-4427-A912-249327502705}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17145" yWindow="4275" windowWidth="15525" windowHeight="9420" xr2:uid="{153C2BD7-A587-4EDD-BD0C-EDF070D407E9}"/>
+    <workbookView xWindow="-16665" yWindow="6765" windowWidth="15525" windowHeight="9420" xr2:uid="{173E77BF-1933-4E8D-9489-CB4F2356690C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -111,634 +111,634 @@
     <t>hash</t>
   </si>
   <si>
-    <t>27226d54c5463327b7303d241b4085e06d976068</t>
-  </si>
-  <si>
-    <t>cc5f8b72ca64287ca8c7ee2071f86f48291d27ef</t>
-  </si>
-  <si>
-    <t>32ea905bbeb88da72e0bca10236f3cbbe9e47124</t>
-  </si>
-  <si>
-    <t>95484818cf046120d00bc872594bab3ff9431f14</t>
-  </si>
-  <si>
-    <t>fada4df892b3bd7257669259894582172625058a</t>
-  </si>
-  <si>
-    <t>a67b004c54c9a42029973cc56d02b15d6a63f471</t>
-  </si>
-  <si>
-    <t>fc02a1b68d8e6a6ad711494b3871a4ade9e5156f</t>
-  </si>
-  <si>
-    <t>2bdcf7c4ded602ecdb20af7b84694988673ce83c</t>
-  </si>
-  <si>
-    <t>d6a2daad7a37ce71ab40e8a670f6ca61765dad3e</t>
-  </si>
-  <si>
-    <t>181d29ccad420dcc5ecf035fbadd6c8bff6a45f1</t>
-  </si>
-  <si>
-    <t>59780e1943ed8046d8029bc49ac49c813d7db756</t>
-  </si>
-  <si>
-    <t>895f8c7b6d072b24473332ff0517b2cc21b77cd2</t>
-  </si>
-  <si>
-    <t>aa1d464f619c6b119fd9cf04e788abd432acd1aa</t>
-  </si>
-  <si>
-    <t>e55fd41a703920d86bc68aea58723070ae6aa55d</t>
-  </si>
-  <si>
-    <t>f152b4c5d91fd5e1002ee60fcf7464e6b1a4f31e</t>
-  </si>
-  <si>
-    <t>4ff524c682a0d0c516d0cb70f51aeebbf4622a7a</t>
-  </si>
-  <si>
-    <t>bea2414c6d2501295cfb140eee1af288f2b8e546</t>
-  </si>
-  <si>
-    <t>a4eb67de6b9b4782988675ec86b0cd4aa67a77aa</t>
-  </si>
-  <si>
-    <t>c21064d9bfa794b4f5227b2c40809512a0b6f5c4</t>
-  </si>
-  <si>
-    <t>0d259e0f684e0b1988f9eb7bcee0a36c9def4130</t>
-  </si>
-  <si>
-    <t>dead5404a418b65c5a16c690a1c30953ec16f835</t>
-  </si>
-  <si>
-    <t>9aec2e62d1721c947a2f366a9457a26a4e63339e</t>
-  </si>
-  <si>
-    <t>5ee36d4fae9e1c0dd76ddc10bb59ec9a82dbeb04</t>
-  </si>
-  <si>
-    <t>3de1b7d80296a289c6ece37ce5f2dea9c9377718</t>
-  </si>
-  <si>
-    <t>3147afc8e522f9e4d691f9b8dee10f3ba1fe0f9c</t>
-  </si>
-  <si>
-    <t>cd963e8918b36f5887db1189084d5483082bd273</t>
-  </si>
-  <si>
-    <t>8807270898558304ba407546da47a9a6779480b0</t>
-  </si>
-  <si>
-    <t>d131f06781faa33bddef62911a5a6aaeb9bb9539</t>
-  </si>
-  <si>
-    <t>56396b06b45f71cc52b6d303e9d66e9486f55277</t>
-  </si>
-  <si>
-    <t>a29e25fefb071dbc19a78567a98c5559e9d5aef5</t>
-  </si>
-  <si>
-    <t>29dcacfaec6b6bdde444fbc2a1ee7ab8779460a1</t>
-  </si>
-  <si>
-    <t>db8294aef82abcdde0e2ff6cc6d6ba6d0dcbcdb3</t>
-  </si>
-  <si>
-    <t>214707223104e067c1816a2876560ec4d986ac84</t>
-  </si>
-  <si>
-    <t>0ce5fe7180b267c961acfb591deb1e51ebfb69e8</t>
-  </si>
-  <si>
-    <t>750a60c73328cb434289d8141965fcb44c1d06ab</t>
-  </si>
-  <si>
-    <t>fd501d0108a2be8fb85183fd4b76dc73fc6473b8</t>
-  </si>
-  <si>
-    <t>0deef74b0af27bfcf933468c4534a313263a3abd</t>
-  </si>
-  <si>
-    <t>0638f0767938324be034643219260e0fbbefb65b</t>
-  </si>
-  <si>
-    <t>747482e04238a33cc093c05bf9cacb60a9a3e5c0</t>
-  </si>
-  <si>
-    <t>31dd6fbcbe1a220d080002bf36da497034e0f93e</t>
-  </si>
-  <si>
-    <t>97fb06eceb95c1daa1460f208f8258a2a9dd734f</t>
-  </si>
-  <si>
-    <t>2fb9e6317b1cba8b5cf4b4320b7c1234e4e64f76</t>
-  </si>
-  <si>
-    <t>989875276abdc7be0c40ab812902c308a6bb221f</t>
-  </si>
-  <si>
-    <t>5e5fdde47c1ed7ff75da396c85f8ed34411f3945</t>
-  </si>
-  <si>
-    <t>3318df2a93cbfb5dcc8c55acf5f9638de06d1ede</t>
-  </si>
-  <si>
-    <t>1a1c7464d3205c753b96dbbfb5a5e598f70e72df</t>
-  </si>
-  <si>
-    <t>22caeb3003ef06c023c547f6f06ec93c5dce8534</t>
-  </si>
-  <si>
-    <t>c82af79b9d6ed3e143092af22378768a267e42b4</t>
-  </si>
-  <si>
-    <t>011c0b31a51b584514dd59cd749d5ca115d2f8df</t>
-  </si>
-  <si>
-    <t>336bedad99608cb7f07da05e2131044a4718b28c</t>
-  </si>
-  <si>
-    <t>172c00c2bd7f0714b8b82d42071b9a123b0857fe</t>
-  </si>
-  <si>
-    <t>10bbf140516e4fe4383de91ee4e467cd815a4c74</t>
-  </si>
-  <si>
-    <t>79548064fbb291a35d9b7cade7ab70fba892ab93</t>
-  </si>
-  <si>
-    <t>195d8b1ed3cf76da8d2555b71b8a29aad719436a</t>
-  </si>
-  <si>
-    <t>fb50d903872edbfef41245b1c0acfe140cbc12e9</t>
-  </si>
-  <si>
-    <t>2912e086bd4648f80928a5f4c7d3f2c4a8689bb7</t>
-  </si>
-  <si>
-    <t>01a83d3e0f14fcb4a08e7d7679f6dc4659b7025c</t>
-  </si>
-  <si>
-    <t>77c0e38334e6858526054af39e2587404d6621c8</t>
-  </si>
-  <si>
-    <t>747376bb0bc6a9aca101b9587fba5b0719c7986d</t>
-  </si>
-  <si>
-    <t>e648d22c46abaa043b1f103a7135dcee6c5704c4</t>
-  </si>
-  <si>
-    <t>d9f13224de6211fae89591131a4fc2a2d92a39a8</t>
-  </si>
-  <si>
-    <t>e1d862b05869749d0b04b5de4325192d08b54f74</t>
-  </si>
-  <si>
-    <t>1f20506c6357eac2876015532c26bffac617a985</t>
-  </si>
-  <si>
-    <t>931eec076ce327117583a69520cf527d0be0a2ec</t>
-  </si>
-  <si>
-    <t>bdf0ea81007191ff08773bfddefa67c92cbed654</t>
-  </si>
-  <si>
-    <t>2ee7e9279d8f28ea6c743c83441adfc69a09fa31</t>
-  </si>
-  <si>
-    <t>37db260423f5103f9a77053f10f8bb3d930d72aa</t>
-  </si>
-  <si>
-    <t>babc2e3ccfd99f5e34292b9ae93fea8606be48dc</t>
-  </si>
-  <si>
-    <t>eba4c7442ddfbf8a432961c04129ccbf1d46b065</t>
-  </si>
-  <si>
-    <t>79e82f6cd73fe7875d91b1843c36be532011c6a9</t>
-  </si>
-  <si>
-    <t>ecc4458e488b58af29ca5aa8a0d22b1ed4cc46fa</t>
-  </si>
-  <si>
-    <t>1d754d00611a3a28838cdf9500b302609990948a</t>
-  </si>
-  <si>
-    <t>a424400e19fd86b92f4921f49e1ee00aa50b0454</t>
-  </si>
-  <si>
-    <t>c1053018a9d639bbbf1d9558d012a30d97cba4c7</t>
-  </si>
-  <si>
-    <t>c948f4d248d3e02fb44e5f9195ddd096f0cf8398</t>
-  </si>
-  <si>
-    <t>7461f8eb6cc5cf092e3d4d4209c3642ca9d70e39</t>
-  </si>
-  <si>
-    <t>8747da35e18a3612f7f383553e7826c3b14f1cb5</t>
-  </si>
-  <si>
-    <t>f933836ea2d87c18771c264ab999a7010bc003a8</t>
-  </si>
-  <si>
-    <t>eaa5426224289058cb362f2de2e3bf6c732ea7bc</t>
-  </si>
-  <si>
-    <t>3b36ffcab758380f44c185bd24a1d89fba058945</t>
-  </si>
-  <si>
-    <t>1a7b398682ce851c007692a99d807550ac6cc4fb</t>
-  </si>
-  <si>
-    <t>b8f00df23978c234fefc27e364030d46e08226a5</t>
-  </si>
-  <si>
-    <t>0a4422d298f9f68d1dafbfb382f9683bf6776532</t>
-  </si>
-  <si>
-    <t>727dc4fc1e76e435c9723ffeed3d07e75222fb69</t>
-  </si>
-  <si>
-    <t>47957cf164d7c400866e7de27481ce3f1d0d1825</t>
-  </si>
-  <si>
-    <t>213fd6f409cf1981b64ae4a4ff2f025848647d65</t>
-  </si>
-  <si>
-    <t>d2321ff7d83566e6d3f7f8253abfbf4fb3277cbc</t>
-  </si>
-  <si>
-    <t>dce01c26ea940d94a3de059b262bf8099d50a4dc</t>
-  </si>
-  <si>
-    <t>6ec47193fb1a0cf1bb1c8a8019543f22c55e901e</t>
-  </si>
-  <si>
-    <t>eec928365896180b7a7fb92f99b775992a16707a</t>
-  </si>
-  <si>
-    <t>564804e88ccdcc33e8d4efce678d62c3addafd30</t>
-  </si>
-  <si>
-    <t>d33d9fa333f61c92a1313dd593d1c4d38c50a8e4</t>
-  </si>
-  <si>
-    <t>b5b75c013f8b08c27ea472fc0a6391b102ab6681</t>
-  </si>
-  <si>
-    <t>03629be8ef2e1142539668954cd44bb9bc988609</t>
-  </si>
-  <si>
-    <t>97f9848402e37e7d90464b2be935e713377dd07f</t>
-  </si>
-  <si>
-    <t>7dd4468487242b29fd6f7a8af79aa136d46bc3e2</t>
-  </si>
-  <si>
-    <t>a022a6aa6e12ea09c0a2bdb8bd033a9480529b89</t>
-  </si>
-  <si>
-    <t>a180b965096d56888576227023238d4d9cbdf82d</t>
-  </si>
-  <si>
-    <t>e03d3f11f8725820da1bdcce686d8fd91e0b656e</t>
-  </si>
-  <si>
-    <t>5ccc80e680da44f84530a3ac094f97a653863dc5</t>
-  </si>
-  <si>
-    <t>32e4a107c14f2b81eb221ee9ec7e86df7d7954b4</t>
-  </si>
-  <si>
-    <t>47791d5c647f21b46a1cc7b835530a5d27a90816</t>
-  </si>
-  <si>
-    <t>2c96597a922f09b4b6e6e8d5c822e6d77367cf53</t>
-  </si>
-  <si>
-    <t>b11d910359b088d912cf4ba8c8776b1e9837a67f</t>
-  </si>
-  <si>
-    <t>bd6fae53d810e4fbc22d9501532bfd5187962cbd</t>
-  </si>
-  <si>
-    <t>12a4f645e8bb0e192f744f9061d54d8adf0ab467</t>
-  </si>
-  <si>
-    <t>87a97e63aac23fa9e7fa012f113c5c2ac828eed8</t>
-  </si>
-  <si>
-    <t>37328025d04b4d3b8b345d3d88dfb67abaa15960</t>
-  </si>
-  <si>
-    <t>85ce398616a71d32c1714d5862266064ddc33655</t>
-  </si>
-  <si>
-    <t>6b8272060756f78e17536a846767d19918a5ba62</t>
-  </si>
-  <si>
-    <t>c613a726933479e1009a2b63126105bc844e949b</t>
-  </si>
-  <si>
-    <t>7d0b8145a53f609727588a48d997a4930ea757ef</t>
-  </si>
-  <si>
-    <t>4223ccc03825644d2bd2d434cf9d0fba723cd7bb</t>
-  </si>
-  <si>
-    <t>275b8f2ff88ae2bfbc2e2b27db318e1a5633ea8c</t>
-  </si>
-  <si>
-    <t>a0542a2575a92b80ce6a97c861e6ea6ab2564933</t>
-  </si>
-  <si>
-    <t>23ffbf7f0aa348b8869020019ba77be422bb53ad</t>
-  </si>
-  <si>
-    <t>a26ff061c1dba8cac1b4f2d3a14b10bd16163816</t>
-  </si>
-  <si>
-    <t>7f3a8c3818d4ba404d3de31d31594f7b673e3078</t>
-  </si>
-  <si>
-    <t>847ac0384703c6e3bfa3892cd48ea7579699cbb5</t>
-  </si>
-  <si>
-    <t>01f748e0a64ddf3d1c245a13774f007a106fbe6e</t>
-  </si>
-  <si>
-    <t>ae307712789e5d497c34deed8e18a7619d111e89</t>
-  </si>
-  <si>
-    <t>ab2513c1d18e4b8562db8849e6751fe86ddb2370</t>
-  </si>
-  <si>
-    <t>58a9ab4df045b70125ed249d8412cf496c1b0a85</t>
-  </si>
-  <si>
-    <t>c75d82fa07c9b4e543da609a37e9da5540d3daa5</t>
-  </si>
-  <si>
-    <t>88557d0b178304a23b2d02b556c4dfb6ed2a7f3b</t>
-  </si>
-  <si>
-    <t>f8ef84c8d252162fcbc9d39bf8670aa63deb1650</t>
-  </si>
-  <si>
-    <t>1df9436465f0dd34e9c8204952e9dc58eb3bd7b3</t>
-  </si>
-  <si>
-    <t>f599d960684ecd4f468c94085e28c8cd2b003a4a</t>
-  </si>
-  <si>
-    <t>8205dd365947beb7bfb353c41ef3e1a83adc32b4</t>
-  </si>
-  <si>
-    <t>13a53c770ab480bc557800df50fa512f3f5a7729</t>
-  </si>
-  <si>
-    <t>d5a9f88d7624d4ff26a3dbae63c6549a499c11eb</t>
-  </si>
-  <si>
-    <t>b1cc263c7eee30588931a9a5590d0eb2aa023864</t>
-  </si>
-  <si>
-    <t>3e2170c3633c91e3abf0a7ec5cecaa5356426b53</t>
-  </si>
-  <si>
-    <t>a0a709c55fa30b1372b4cffe85df71f30caa3899</t>
-  </si>
-  <si>
-    <t>d8ba03398c0d1445fc4294566fb0f320e216ec0e</t>
-  </si>
-  <si>
-    <t>528c81d71aac2e815dd5f97f93094790519df301</t>
-  </si>
-  <si>
-    <t>af3e3a734ca58d8aa3580c0481122ab8dee86822</t>
-  </si>
-  <si>
-    <t>9eaf608c43b027d7373adb6ce85431057743246b</t>
-  </si>
-  <si>
-    <t>536a077e1cf0d90220ee0ad69fb5bc340893acec</t>
-  </si>
-  <si>
-    <t>f8cd158b8e43dbe929f56b603b58e7b13d54b26d</t>
-  </si>
-  <si>
-    <t>5c7547068fb930cc3f6b3b441cd340a715ae4779</t>
-  </si>
-  <si>
-    <t>e37ae067ed0e7f928f4b8999549347bc7f7de1e9</t>
-  </si>
-  <si>
-    <t>e0314a5e75a442dd59f157cece1c3fad4e8a2816</t>
-  </si>
-  <si>
-    <t>0839f4e2f3e4eb1903006caae88a6b94d698cff0</t>
-  </si>
-  <si>
-    <t>5f5e41bb6cadeba5abfd68802682b46ad0cc9744</t>
-  </si>
-  <si>
-    <t>f2dfde6e32221cfc6121cea8face4b2d97155b31</t>
-  </si>
-  <si>
-    <t>2265ba775add66aec3db7bd0a2d1ce526ce8665b</t>
-  </si>
-  <si>
-    <t>beb54ed2826779c70a982e6dc0c979c4d353632e</t>
-  </si>
-  <si>
-    <t>c660e122414214b86c3edf4d8118a57ea2e7e5ed</t>
-  </si>
-  <si>
-    <t>6389a9d4b7497270c0c6358bbe50444cca382251</t>
-  </si>
-  <si>
-    <t>94dc560965d6e9a3634ff88c7f87cd4d694213b3</t>
-  </si>
-  <si>
-    <t>f8659c0fbe45fcc837bfa5d4b7f08190d50f004f</t>
-  </si>
-  <si>
-    <t>58717f6e34df4edf3cf7151f70a317a9df3fe502</t>
-  </si>
-  <si>
-    <t>75f6ec6c5466ab28ebd478491a3d9e5170e00ac0</t>
-  </si>
-  <si>
-    <t>b4e1dc9dea7c1264e564734c87a30fca95acc48f</t>
-  </si>
-  <si>
-    <t>05cde73c90ca0ed6662443806bac8ed0c88ad0fe</t>
-  </si>
-  <si>
-    <t>6bf618334e05890b5c4f9cda01ffc2295a61ed87</t>
-  </si>
-  <si>
-    <t>42f157bb4183cb6bea6e2e6a131ad3e78854c32e</t>
-  </si>
-  <si>
-    <t>463d9263454c43802c3304ca8ada6943a5e53810</t>
-  </si>
-  <si>
-    <t>39208e86a8c34bb1c2b97acdd5a1e5e8f2360f50</t>
-  </si>
-  <si>
-    <t>0ac10c9611c4e6df705ad3b5eb41d69a818d4920</t>
-  </si>
-  <si>
-    <t>ebab58dbeb57d7c687493e1ab1306e0864a0ece7</t>
-  </si>
-  <si>
-    <t>7aa14b40f84bbccfb3fc52ef8b688f15e333e0ea</t>
-  </si>
-  <si>
-    <t>4e64c44f3416bd1c1b82b670f57b9cc5587e87eb</t>
-  </si>
-  <si>
-    <t>f72be29e3f0f3652e7faed65c85c689bc9b2c85a</t>
-  </si>
-  <si>
-    <t>cc93262abb8c1063e950228ff199ba5d6c646beb</t>
-  </si>
-  <si>
-    <t>b9bfbb0b0906c42377f8854014aa462e05b730bb</t>
-  </si>
-  <si>
-    <t>2ee58a56915568c6c1205f604256ec7b32b71ad3</t>
-  </si>
-  <si>
-    <t>74af25b358b114b519f2ed11a878831962df1e6a</t>
-  </si>
-  <si>
-    <t>bcb54c8404ec3907e2ba5932a3db0415b3ff8c63</t>
-  </si>
-  <si>
-    <t>c03b719c796ec5975da73eb7e92b3203c43bcc30</t>
-  </si>
-  <si>
-    <t>c6e2e04657c1faac443d23b3f750dc1d95bb4a32</t>
-  </si>
-  <si>
-    <t>1e738f9ad87eec239222e83463c51ff302fa99e8</t>
-  </si>
-  <si>
-    <t>50d436dc00f62815596ca9dbfcb34806fe37ad2c</t>
-  </si>
-  <si>
-    <t>31d498ae1567500996d42422b132eb405c0b967c</t>
-  </si>
-  <si>
-    <t>941e45777280479af34f74d890ab0bb12e1c441d</t>
-  </si>
-  <si>
-    <t>ef5e1a6967e47132a3bb6ff8a2a32f8c09d889b3</t>
-  </si>
-  <si>
-    <t>ef22baaf72eefa0edefd52da0b0d9b895d510db8</t>
-  </si>
-  <si>
-    <t>542bdef3b7b6c08b15f202ae8a79496a04cb43c1</t>
-  </si>
-  <si>
-    <t>d0995a347c52475bae12b0fda55cf32e53c66cd3</t>
-  </si>
-  <si>
-    <t>d7b6f1393029391750cf6a1401423c3ec99f0ec3</t>
-  </si>
-  <si>
-    <t>f448fbc359c19d14900b57e38ef9520425e0c4d7</t>
-  </si>
-  <si>
-    <t>f8e18c50808a6ca5ae5d02c9ab77575202071c3f</t>
-  </si>
-  <si>
-    <t>4f1c28ced8bdb2eeec6e2f59fa53ee654f3fad29</t>
-  </si>
-  <si>
-    <t>52efc7601facfd2108a15f1c0ea837e7e7dda7f9</t>
-  </si>
-  <si>
-    <t>47d4b82614dca4f8438563805bb89d37250e6c03</t>
-  </si>
-  <si>
-    <t>656f158be2da965b92c0f5106eba9c00a612f667</t>
-  </si>
-  <si>
-    <t>f69794a47b48dbd553c15088248ba9a70d9da636</t>
-  </si>
-  <si>
-    <t>78d61e46384dfe83de6f90b67b288ad17548b2a4</t>
-  </si>
-  <si>
-    <t>3ea013bdb5e1f175d3e7fde8e92aef06b6c63814</t>
-  </si>
-  <si>
-    <t>4aebf4f271d226588f0f6067bd376d7a473acee4</t>
-  </si>
-  <si>
-    <t>f1871be6a8ba19ec2f12f1c11ec47a9bbefd823f</t>
-  </si>
-  <si>
-    <t>a036cbc97374a0d9f5340db02fcf012872995a5f</t>
-  </si>
-  <si>
-    <t>0c2a9cf03604059bac959fea5d4a560f30cdd88d</t>
-  </si>
-  <si>
-    <t>b348e7d6ebecf27847b02bcd0857e4d0e5102479</t>
-  </si>
-  <si>
-    <t>e46d1394da8da02c2c81e090696232215ce6f777</t>
-  </si>
-  <si>
-    <t>86df4357fbc522100e689ac7ba1963986afc2ced</t>
-  </si>
-  <si>
-    <t>9ae5ccff7711a0ae68249777ef09a8718c1ac6df</t>
-  </si>
-  <si>
-    <t>7e09cf716fa15f3a0a790d3490865fb0637d15a1</t>
-  </si>
-  <si>
-    <t>3e9f0f9ffec9aaab2a4f7edf1e2e18a3937f9f7e</t>
-  </si>
-  <si>
-    <t>7c6f7b01232e2496e9dc0e44559cf0a77d418396</t>
-  </si>
-  <si>
-    <t>cd5b84e7603f61efa8da39215f58a8fc8ebcdb16</t>
-  </si>
-  <si>
-    <t>3fb967d40d0782b54ba8562fca60b4af9f0ae3e0</t>
-  </si>
-  <si>
-    <t>c1345b14b94ddcbbc28a811c633fc014ba202c74</t>
-  </si>
-  <si>
-    <t>9895671edf70c4e47d516f1899b859acfe1a846d</t>
-  </si>
-  <si>
-    <t>b381094327f215174f4ba7c7501775803403cac3</t>
-  </si>
-  <si>
-    <t>3ce624644eb8e00db06de029d9dd91564102073b</t>
-  </si>
-  <si>
-    <t>3a0acd9dfe3240ad72059bb1e3647f0c6fc6ea87</t>
-  </si>
-  <si>
-    <t>05a0bd8fecfd9dc8b811fcab3cdc94a48203b74a</t>
-  </si>
-  <si>
-    <t>362d9aab797168b7a44343c8d19463c329a61f14</t>
+    <t>778939c85038d44a9971febca159642f855dbc36</t>
+  </si>
+  <si>
+    <t>799178372e22c5acb8461bbf782da9589ea9b46a</t>
+  </si>
+  <si>
+    <t>6032658be59e09b9eab2a140028a1e4a74ba156c</t>
+  </si>
+  <si>
+    <t>4b4643c2357f74bddd753d09415157057db66377</t>
+  </si>
+  <si>
+    <t>6ea9414f76a906223fe539a2da44409f30bcf875</t>
+  </si>
+  <si>
+    <t>2caa1900e8e8a6b66772bca23b277c49b7456e02</t>
+  </si>
+  <si>
+    <t>ca852a14192667640a9c6b7562908d2b4e0e6676</t>
+  </si>
+  <si>
+    <t>6d2d262dabf31646877e0531dbd541bd3ba7a02e</t>
+  </si>
+  <si>
+    <t>399d14d51de77b7e71c9107b4868330e87bd341f</t>
+  </si>
+  <si>
+    <t>76570ecf622e30b9f150e7327bd82a45045f8e47</t>
+  </si>
+  <si>
+    <t>005d512d5734e2ea7cda5119fda3bcbda43d8505</t>
+  </si>
+  <si>
+    <t>9ea199154adf335a2e091c363156f5ea086672a8</t>
+  </si>
+  <si>
+    <t>90ac2128f0c5a7b12a30f70bef67761edc974129</t>
+  </si>
+  <si>
+    <t>59e35c9d75e8d81e2f3322fa124e3c9e2df0656b</t>
+  </si>
+  <si>
+    <t>180860cbfb23f177088458a6f34c327a2c6c8c9a</t>
+  </si>
+  <si>
+    <t>91a52d93d4a33cb01d2c59fb4bc1d6171e0b1dfc</t>
+  </si>
+  <si>
+    <t>6e96e888a90d61fb40868c34f055f90ed23ddd31</t>
+  </si>
+  <si>
+    <t>462d2a282dcf101f75588d0248fb350969633bfe</t>
+  </si>
+  <si>
+    <t>bf1ef4648fb6b8498ac75e1bf373bbc160309272</t>
+  </si>
+  <si>
+    <t>ddb5a91427c443653c9aec4493d93484dbd5f1ec</t>
+  </si>
+  <si>
+    <t>4ab90964bf72d1a28725a21b2e7d84c288065edb</t>
+  </si>
+  <si>
+    <t>80aadea2fb33353d0127db40f4ff7c9a8bead987</t>
+  </si>
+  <si>
+    <t>a0a1acd9744fe491e7b3e5263197b0816b6eb8fe</t>
+  </si>
+  <si>
+    <t>6a74d12e89daebf72eed887750e153b833d46e0d</t>
+  </si>
+  <si>
+    <t>c8500c002cc264d04f1d0e989753bf328145a8dc</t>
+  </si>
+  <si>
+    <t>2c93bde4eef11258eb719d2816b32dc3ab63a021</t>
+  </si>
+  <si>
+    <t>c0db62107d511d1b7e337c718448384df5ec8146</t>
+  </si>
+  <si>
+    <t>f4df73c036f16b900d9d6ed5911eb11db356cb5d</t>
+  </si>
+  <si>
+    <t>e66cbfc0dfc726a09d6445e28f4d0b83ec5c1b1c</t>
+  </si>
+  <si>
+    <t>0c317cee3f6fce6ae077d0eb1743d5804fe62eca</t>
+  </si>
+  <si>
+    <t>1f3ad865dea88d9197cff090862a2b50be4106db</t>
+  </si>
+  <si>
+    <t>34deabb480e266924485433a1e0084142d1ec78b</t>
+  </si>
+  <si>
+    <t>3b8dbec78ded8d1550a9741ad8d5fd7db35114d4</t>
+  </si>
+  <si>
+    <t>6d2c3d4abdd4a2045c068f7f5af8aafffa4d4b13</t>
+  </si>
+  <si>
+    <t>e82a5d19173016c65a52ee2cb60d5cedacb284a5</t>
+  </si>
+  <si>
+    <t>e4154b1a6c80c5b04473e3ef0360a029fb69efb1</t>
+  </si>
+  <si>
+    <t>0b65a679ab78b98fd861fe3e955c38af230e9aa4</t>
+  </si>
+  <si>
+    <t>e13b3f18b40a837f59d5d34301eedf0e9d892409</t>
+  </si>
+  <si>
+    <t>d25a95ed5ea5cced2ac6af0a8cedc6c02c74670d</t>
+  </si>
+  <si>
+    <t>c353c42f8f7005dd0228ee303c9cba1b9409c915</t>
+  </si>
+  <si>
+    <t>8dce3a04b5190c2c4b1af629b575f8bcd8c7bd3b</t>
+  </si>
+  <si>
+    <t>469fca992f737dff41cdb6140fc9a27e238538f5</t>
+  </si>
+  <si>
+    <t>6fe783529d803c43e7dfc0bd6639f068d54e2e1c</t>
+  </si>
+  <si>
+    <t>4c6419530878a1763f1e7629fb44f7bc3d12e98f</t>
+  </si>
+  <si>
+    <t>1e6645a490f395a9aef04871ee8ddc469b8d8b54</t>
+  </si>
+  <si>
+    <t>aa60f7d1fa3239c18700b79387230fb93bb1464f</t>
+  </si>
+  <si>
+    <t>828de963ec7c089e29a2224c3714b986cd24bc91</t>
+  </si>
+  <si>
+    <t>15e7b6feca9f3d44ed34d060f9a7b9986b055684</t>
+  </si>
+  <si>
+    <t>239def7c47847b579fe6763deac915b9d7ac2af4</t>
+  </si>
+  <si>
+    <t>bcfcc626c89ea19eb56216074ae7b343ba3d6854</t>
+  </si>
+  <si>
+    <t>233d5c49316137c9295abfab20aee4ee3bfa2998</t>
+  </si>
+  <si>
+    <t>7a479606ca94889c4329df4da0ac9c9c83da8617</t>
+  </si>
+  <si>
+    <t>d2654aff6f508e38a12893dbe6b6d023d790b898</t>
+  </si>
+  <si>
+    <t>883f74f3fcdf739134589041916dd2fc4e6e73f8</t>
+  </si>
+  <si>
+    <t>fd0450f157cc2b1481653860e62833e0d61a303e</t>
+  </si>
+  <si>
+    <t>bacc8cfc95875f07c82758743013300490615ade</t>
+  </si>
+  <si>
+    <t>4e75e13ae0f1723f2d992724cf188c97c85b379d</t>
+  </si>
+  <si>
+    <t>e8d036ab4e733b8a5a25d6351727d71ee94240a0</t>
+  </si>
+  <si>
+    <t>29058506ee88e495c9129d2cb0f238bb666f188f</t>
+  </si>
+  <si>
+    <t>27af68e72e8771b67cb3cc195a764c1dc717b7fa</t>
+  </si>
+  <si>
+    <t>c38adab242672b897df2f111eac72487967b9c73</t>
+  </si>
+  <si>
+    <t>bc3f0bb57cabe946238bff47f6592c36abeb6cdd</t>
+  </si>
+  <si>
+    <t>4b9c2b34157b959fabb26b920039476ea6e2fdd5</t>
+  </si>
+  <si>
+    <t>b94940898d1c08880e23a6aaca121954cf103228</t>
+  </si>
+  <si>
+    <t>a660e588097cb214adef691bbfe96ac1308d86e3</t>
+  </si>
+  <si>
+    <t>9ccec1c8dca79a8fc0158495057e28d2c76d1b7f</t>
+  </si>
+  <si>
+    <t>c95369643ea0dbc7fdc27cf612e1ab6cc8dc6ae3</t>
+  </si>
+  <si>
+    <t>08c17637cd327df3f26a166b2b483e9adf89aade</t>
+  </si>
+  <si>
+    <t>6f73ddd438276f8e4494e207b0ef67e3b49ce9df</t>
+  </si>
+  <si>
+    <t>e652d0d7df30b1639c62e9430c78dba1284a390c</t>
+  </si>
+  <si>
+    <t>5d2cf54488b09ad4c9bcbe30e50155dcab73d435</t>
+  </si>
+  <si>
+    <t>e80f671a51486f609be7ecd36b9cc6e915e4c5dc</t>
+  </si>
+  <si>
+    <t>987ed09f0283960b7a03c2a1e504d4c98b9d6625</t>
+  </si>
+  <si>
+    <t>b9c29f279a0d6a10dcb9890386915ddf856009f0</t>
+  </si>
+  <si>
+    <t>4e478c81aae044def46873837ab882b24695b6dc</t>
+  </si>
+  <si>
+    <t>052c4c0ae59bee2da5ddaa762e5dcee394f3bd02</t>
+  </si>
+  <si>
+    <t>b736c7f359ced4a16c083e8ce9c688b3aaa40040</t>
+  </si>
+  <si>
+    <t>f8a632c31859ab52af152017ab19f436ccc27e03</t>
+  </si>
+  <si>
+    <t>9332161caa6153e78e72de4f62d9830c2ed61895</t>
+  </si>
+  <si>
+    <t>6312d60a3ffd863b42ebac88c0f88d91b42d59ac</t>
+  </si>
+  <si>
+    <t>9353b82523fe821890a68defa7308469fafb7990</t>
+  </si>
+  <si>
+    <t>a9cf106c6e1d5a60dcec34a3259a0a30efddc74d</t>
+  </si>
+  <si>
+    <t>28fc9734fad62ff6a5abcbb190a7fefe78c3e559</t>
+  </si>
+  <si>
+    <t>635a180fe24ab2f09b35b79d232c3b935689089f</t>
+  </si>
+  <si>
+    <t>623ef982f42ee075f2c5aa0b0930e7952fb17d76</t>
+  </si>
+  <si>
+    <t>de1e0807d4d85eea84862695d23210c4252f9178</t>
+  </si>
+  <si>
+    <t>9c5d7aa23a474aeef46c298299d55eef5d5d217e</t>
+  </si>
+  <si>
+    <t>7f790351c9122a6e48a858f70f43a6d11ae91505</t>
+  </si>
+  <si>
+    <t>f0f5b9caef2a6616bb3636e491aaf3b0662312dc</t>
+  </si>
+  <si>
+    <t>b6cb79d4de380059ef046b36b45e20fd2f839be7</t>
+  </si>
+  <si>
+    <t>1d67481acc59364fcd948edd533ec42eb63601ac</t>
+  </si>
+  <si>
+    <t>a44dc86dedc70238e7a5992a1a4905fbaa741bf0</t>
+  </si>
+  <si>
+    <t>3d69536212b24af05db66c41a8a654e172afe768</t>
+  </si>
+  <si>
+    <t>6633f2f701d805a3f4f044906b4ff66b9ce93164</t>
+  </si>
+  <si>
+    <t>f92d34ab192a4264ae72dd948f57c4443a772657</t>
+  </si>
+  <si>
+    <t>1fd265e79f49663b84b9e6b4c5b1c16f7961fc84</t>
+  </si>
+  <si>
+    <t>3f62144d9652d4ce4f7a6dd38a21636e51ed3ac9</t>
+  </si>
+  <si>
+    <t>cf0332d8133a7bbe429ac4ab5d111bd22ca2a985</t>
+  </si>
+  <si>
+    <t>9459dde6cba7585ebaba42a22a598a5b9a0076b7</t>
+  </si>
+  <si>
+    <t>376e77ef5afe968e04acbc69321361177f6a1b63</t>
+  </si>
+  <si>
+    <t>4231b3d2cefea0ba347170f556e7bd3858ee1870</t>
+  </si>
+  <si>
+    <t>b7b5a6d650c203b84fbd5c3243265ee09efe74e4</t>
+  </si>
+  <si>
+    <t>f7d3cddf479d8b4d0a175a9d216341275cf158c5</t>
+  </si>
+  <si>
+    <t>0b7ce11ff75e51cba5534f6c23657284751548ac</t>
+  </si>
+  <si>
+    <t>b57c945e020a4d76fc4f3c3fac4a746d95491033</t>
+  </si>
+  <si>
+    <t>dc598d457d076011d4930253196c9e2029403e19</t>
+  </si>
+  <si>
+    <t>092c0c129b6fe408afccb235add6c5c343d91aef</t>
+  </si>
+  <si>
+    <t>a2777dc0a0f8fa0473796b00ab7205c7b9243618</t>
+  </si>
+  <si>
+    <t>f0a314199c3136cf26bc2ce79cd600dd1f1ba9a2</t>
+  </si>
+  <si>
+    <t>dff3d169a5177021dd40881f1944f8b7c1d3e123</t>
+  </si>
+  <si>
+    <t>6b0ce7d5612c5f64b7cdd37ab73343bde0e5da51</t>
+  </si>
+  <si>
+    <t>aeef6e4c2e6e284ff774b5fb9a08513689ff26f2</t>
+  </si>
+  <si>
+    <t>4b6a442c5e84099bd532a971c911676621e87a89</t>
+  </si>
+  <si>
+    <t>25dc708d29e290bdc753ed2eb14665f9fbeaf7eb</t>
+  </si>
+  <si>
+    <t>4410fd9d4951e722c62e9acc00646643b3b9a665</t>
+  </si>
+  <si>
+    <t>855d3346790ee59915519fd2e49d485760e34c70</t>
+  </si>
+  <si>
+    <t>33d3543eed49891a3a4dd909955606daa776c2e8</t>
+  </si>
+  <si>
+    <t>ec6da2232ce4cefeef5ef62ae82cb26b7fd84d11</t>
+  </si>
+  <si>
+    <t>2bef36d99ca09d4a45b2f9e953157cb1f2c2c25e</t>
+  </si>
+  <si>
+    <t>665a6bebf9d57fdeeec3631d0ef901c7df82fddb</t>
+  </si>
+  <si>
+    <t>1409ce27c05a138115d334a65f96fb8130074bdf</t>
+  </si>
+  <si>
+    <t>fcba8fdccc1afd9959dcf22f62678e2ac23a5010</t>
+  </si>
+  <si>
+    <t>8fce504777ee50c00452e70fe89839075c366b48</t>
+  </si>
+  <si>
+    <t>6185cbb498e875527f4ec3f2052520b482a118c6</t>
+  </si>
+  <si>
+    <t>c3af4decf1c5025d306f416bddc789fdab6a9fd3</t>
+  </si>
+  <si>
+    <t>093150111d5145fcb9b5695ea8262e730e1ef671</t>
+  </si>
+  <si>
+    <t>9110710ebe17c16892c8eeef78e049c42c94beae</t>
+  </si>
+  <si>
+    <t>d56e73674911033219a0e2fc5d048c00538ef869</t>
+  </si>
+  <si>
+    <t>cc71b9211d53f40d375c0c171d0613c79648255b</t>
+  </si>
+  <si>
+    <t>62141d0bc20b009f71fae771e2e3ea0f1a2a483d</t>
+  </si>
+  <si>
+    <t>a1ef5f542f2cf8af8ff503f481f6ec847865b72b</t>
+  </si>
+  <si>
+    <t>02c2e4a4bf817aae445f2f1eb71bbbc1addc2b91</t>
+  </si>
+  <si>
+    <t>103de7e8816eecc1a95dbc37cdf2382319eef661</t>
+  </si>
+  <si>
+    <t>7a8e1fcbc06952de83d47ea3cdabe37480248821</t>
+  </si>
+  <si>
+    <t>424732751f95502f8c875a4f874ef4d1cc08b4fb</t>
+  </si>
+  <si>
+    <t>da9b9e222d0fa3705f04b4474834b78f02e201d2</t>
+  </si>
+  <si>
+    <t>6e37acaa4ae0120c5bf8b8716387d3540592ad86</t>
+  </si>
+  <si>
+    <t>a424d824156836f94513c2a716a586b3563d2b6d</t>
+  </si>
+  <si>
+    <t>93a2ca52c02d4e8887ece6a16ced7dd33c2fc8f4</t>
+  </si>
+  <si>
+    <t>a2b01ce84c335556d9f2f30a1fe593e83d23ffc7</t>
+  </si>
+  <si>
+    <t>06b90280dfeacc2bcea54704f453e36ae90adc35</t>
+  </si>
+  <si>
+    <t>9c6d8b9586ca77a48e2a719c611ae0091c2a63e9</t>
+  </si>
+  <si>
+    <t>8314a1b47ac328424aaacdf9b2cb3fe71c3bb437</t>
+  </si>
+  <si>
+    <t>c3fd80bf43827ce119d2cfc866b18a73d4888d7d</t>
+  </si>
+  <si>
+    <t>646f84b18c0239d344cabef5dd098608cda3ff48</t>
+  </si>
+  <si>
+    <t>89e74f541df1d822d7a344e376fc2610a0eb53ec</t>
+  </si>
+  <si>
+    <t>8dd0d1d45b6809b99351238d2fb7aea40affbdaa</t>
+  </si>
+  <si>
+    <t>43ccc0bcc8d29619c2fcc8a5c7038cdd686065c1</t>
+  </si>
+  <si>
+    <t>313464b6a4428d87fed860ef30a649a83c0e5442</t>
+  </si>
+  <si>
+    <t>6c00f62c58a47a8b44a56e28b96d7c4068a3f58d</t>
+  </si>
+  <si>
+    <t>eb5f65f782a38270c39cc8e8046e5826cb078379</t>
+  </si>
+  <si>
+    <t>adaf4adf49c45f3b9b1e0bddbd5fbe57045ea6e0</t>
+  </si>
+  <si>
+    <t>fb440786e83eaa8e4f5b5bcbde16a9747ac36c9d</t>
+  </si>
+  <si>
+    <t>bb79aabd131d8c95ab98db646917d787e48dc85f</t>
+  </si>
+  <si>
+    <t>e24354778ae51769316d08e4535a84ac396d37e4</t>
+  </si>
+  <si>
+    <t>eef60f9f755dee08f5249e92a1640c5f6072cfc1</t>
+  </si>
+  <si>
+    <t>2e4bdc9b84d609b40913f9e5cd9ca7316a216553</t>
+  </si>
+  <si>
+    <t>375a09953277c464f6793b87c9a7d284338fb5bc</t>
+  </si>
+  <si>
+    <t>aeec2e892ef7ff13cdb260d81c2486f6939140be</t>
+  </si>
+  <si>
+    <t>830a8f6f6eb44e73b3d92b0370da8ead62a7af07</t>
+  </si>
+  <si>
+    <t>c49ef40e91c51e2d7894ad0027d9b6188ba9cbb7</t>
+  </si>
+  <si>
+    <t>d707a4d4bd09f97c6ad4d2186048817a2b4c5a2d</t>
+  </si>
+  <si>
+    <t>0f4a6d3e6a8e216e1641f938d398defdb3ffbf46</t>
+  </si>
+  <si>
+    <t>6551d8ac255308f4ec945bdd033b40250724eaad</t>
+  </si>
+  <si>
+    <t>aa741fe9e3f66f4b8a3b01eb6141eb1a1d37c259</t>
+  </si>
+  <si>
+    <t>b4149e04b6c9bad408e0b3383c75698d9567e954</t>
+  </si>
+  <si>
+    <t>88397e60fa75bb3681e72a46be7a51c779108354</t>
+  </si>
+  <si>
+    <t>c6329c516741924367a9b2e11d3ee8a0613b31d5</t>
+  </si>
+  <si>
+    <t>6c2bce45530ff6215a9a9b098ab6ffa5923ed708</t>
+  </si>
+  <si>
+    <t>ed751b4dc4044ca4ed902807c197c7706c82f050</t>
+  </si>
+  <si>
+    <t>b3d0b542e64df65fc123846cc5f859388b256409</t>
+  </si>
+  <si>
+    <t>dc66286b45d9bd7df3642f0a1a25f490fa8b19c8</t>
+  </si>
+  <si>
+    <t>a128bb811a4c1a63ba0f3fba391d18967d83385c</t>
+  </si>
+  <si>
+    <t>0b80cf3e80da13b3d49bb31c73e5db3745a4f89a</t>
+  </si>
+  <si>
+    <t>5c27455119fab869c526003af09da8dc33fe47c5</t>
+  </si>
+  <si>
+    <t>944323f37e1b227e465c2748601c05bf12f9c60a</t>
+  </si>
+  <si>
+    <t>29f5440348e4ea9cef6d55987c1b8c897b523db5</t>
+  </si>
+  <si>
+    <t>e21e88e4a587c124e5fa445b7aca1fdd8907e607</t>
+  </si>
+  <si>
+    <t>07a6fc54d7b5ba36704f4b85d01c68da73f9585b</t>
+  </si>
+  <si>
+    <t>bcfa74486c7fc35b341d253c28d7503b5cce006e</t>
+  </si>
+  <si>
+    <t>7c7ddeb3ae118ab305f654aba6a67c79c895cd0d</t>
+  </si>
+  <si>
+    <t>59ac0e41baf6ac4547046c4796a2f1f85c4eb6aa</t>
+  </si>
+  <si>
+    <t>b646ef22a252e8771df6cf7887d1ed866969601e</t>
+  </si>
+  <si>
+    <t>8e1d6d4c86f206c073e0bb54f24f97704775cf48</t>
+  </si>
+  <si>
+    <t>489785deef6ef20ef631a16a563b3cf10757ce99</t>
+  </si>
+  <si>
+    <t>e5c5d83a450c30d74ca2eab64c32e29fec54a986</t>
+  </si>
+  <si>
+    <t>842b3e7f9f913b199aabf891ee1363df3d21cbb4</t>
+  </si>
+  <si>
+    <t>f5016a3253b110f01e6986d20bfe8434ba56a883</t>
+  </si>
+  <si>
+    <t>87a3b0026a394b7386014cda5a7275c7c0465eae</t>
+  </si>
+  <si>
+    <t>c18a22810859e96ab65def73d3fb9ce217e1210c</t>
+  </si>
+  <si>
+    <t>c810b58a4176ce35ed8cb24475cfa8c4cbb8dca8</t>
+  </si>
+  <si>
+    <t>42a54c1bd19242dfb01abeb75208986a5f162fe1</t>
+  </si>
+  <si>
+    <t>d90ece027ee63bc61c1e62882fde41398d04daa6</t>
+  </si>
+  <si>
+    <t>e39e9be90168fbf9350f2c29315841e42476d211</t>
+  </si>
+  <si>
+    <t>677607e806a768435ba28a45669992bf5e8c56fb</t>
+  </si>
+  <si>
+    <t>12bca2ffe0c8fcf4f384c87cd4637e92a25026ee</t>
+  </si>
+  <si>
+    <t>d222f2fdedda916a6497c966d59ea0b048919a6b</t>
+  </si>
+  <si>
+    <t>b00db232d283ef274d4c51ba2387bcdba958336e</t>
+  </si>
+  <si>
+    <t>13a8a8cb5d3cdab820ec8e3c06adeb82f8692b8f</t>
+  </si>
+  <si>
+    <t>83985b69318722eef94708232ef9220357e63e48</t>
+  </si>
+  <si>
+    <t>9c2d828d665e82d94d9c38ce575303d65524c3dc</t>
+  </si>
+  <si>
+    <t>9d1c62132ab64cac3c214ab6ccb24558908966db</t>
+  </si>
+  <si>
+    <t>37d589c1835d469ac18e28e519c8ee3d16cb382b</t>
+  </si>
+  <si>
+    <t>19e828acff66861fb1d1cf39050719b830e33da2</t>
+  </si>
+  <si>
+    <t>e0a391404969f09867249bba3ba0421ef5cd9f18</t>
+  </si>
+  <si>
+    <t>31dbe85b18cbaeee4eba3e5943ce35dfa279e8c7</t>
+  </si>
+  <si>
+    <t>79f85e735416481d3a17d2f5f1e28a651bf580f9</t>
+  </si>
+  <si>
+    <t>5dc88752e083a3e1bb606b30fb6c00f9a0445b44</t>
+  </si>
+  <si>
+    <t>de2f615038a3510925f9ef9aefae52a7c2427b8b</t>
+  </si>
+  <si>
+    <t>a29189477fc385ec2fd0f07f11dacb3d913b8dcd</t>
   </si>
   <si>
     <t>841d8bd48d0e276e2dc66a458dbb38486ec4e643</t>
@@ -1433,12 +1433,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E154205-9C74-4B7D-AC30-C0DDDB012B4A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AB7CDD9-7AF9-4F5F-88D0-E9E904DCB3F5}">
   <dimension ref="A1:Y325"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -1560,7 +1558,7 @@
         <v>44176</v>
       </c>
       <c r="N2">
-        <v>283555</v>
+        <v>284309</v>
       </c>
       <c r="O2">
         <v>603554</v>
@@ -1578,7 +1576,7 @@
         <v>0</v>
       </c>
       <c r="T2">
-        <v>3067</v>
+        <v>3115</v>
       </c>
       <c r="U2">
         <v>4335</v>
@@ -1637,7 +1635,7 @@
         <v>44175</v>
       </c>
       <c r="N3">
-        <v>280488</v>
+        <v>281194</v>
       </c>
       <c r="O3">
         <v>599219</v>
@@ -1655,7 +1653,7 @@
         <v>0</v>
       </c>
       <c r="T3">
-        <v>3088</v>
+        <v>3206</v>
       </c>
       <c r="U3">
         <v>5424</v>
@@ -1714,7 +1712,7 @@
         <v>44174</v>
       </c>
       <c r="N4">
-        <v>277400</v>
+        <v>277988</v>
       </c>
       <c r="O4">
         <v>593795</v>
@@ -1732,7 +1730,7 @@
         <v>0</v>
       </c>
       <c r="T4">
-        <v>2655</v>
+        <v>2661</v>
       </c>
       <c r="U4">
         <v>4309</v>
@@ -1791,7 +1789,7 @@
         <v>44173</v>
       </c>
       <c r="N5">
-        <v>274745</v>
+        <v>275327</v>
       </c>
       <c r="O5">
         <v>589486</v>
@@ -1809,7 +1807,7 @@
         <v>0</v>
       </c>
       <c r="T5">
-        <v>1347</v>
+        <v>1297</v>
       </c>
       <c r="U5">
         <v>3614</v>
@@ -1868,7 +1866,7 @@
         <v>44172</v>
       </c>
       <c r="N6">
-        <v>273398</v>
+        <v>274030</v>
       </c>
       <c r="O6">
         <v>585872</v>
@@ -1886,7 +1884,7 @@
         <v>0</v>
       </c>
       <c r="T6">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="U6">
         <v>2311</v>
@@ -1945,7 +1943,7 @@
         <v>44171</v>
       </c>
       <c r="N7">
-        <v>272252</v>
+        <v>272885</v>
       </c>
       <c r="O7">
         <v>583561</v>
@@ -1963,7 +1961,7 @@
         <v>0</v>
       </c>
       <c r="T7">
-        <v>2461</v>
+        <v>2480</v>
       </c>
       <c r="U7">
         <v>3457</v>
@@ -2022,7 +2020,7 @@
         <v>44170</v>
       </c>
       <c r="N8">
-        <v>269791</v>
+        <v>270405</v>
       </c>
       <c r="O8">
         <v>580104</v>
@@ -2040,7 +2038,7 @@
         <v>0</v>
       </c>
       <c r="T8">
-        <v>2563</v>
+        <v>2573</v>
       </c>
       <c r="U8">
         <v>4652</v>
@@ -2099,7 +2097,7 @@
         <v>44169</v>
       </c>
       <c r="N9">
-        <v>267228</v>
+        <v>267832</v>
       </c>
       <c r="O9">
         <v>575452</v>
@@ -2117,7 +2115,7 @@
         <v>0</v>
       </c>
       <c r="T9">
-        <v>2706</v>
+        <v>2825</v>
       </c>
       <c r="U9">
         <v>5331</v>
@@ -2176,7 +2174,7 @@
         <v>44168</v>
       </c>
       <c r="N10">
-        <v>264522</v>
+        <v>265007</v>
       </c>
       <c r="O10">
         <v>570121</v>
@@ -2194,7 +2192,7 @@
         <v>0</v>
       </c>
       <c r="T10">
-        <v>2733</v>
+        <v>2804</v>
       </c>
       <c r="U10">
         <v>5028</v>
@@ -2253,7 +2251,7 @@
         <v>44167</v>
       </c>
       <c r="N11">
-        <v>261789</v>
+        <v>262203</v>
       </c>
       <c r="O11">
         <v>565093</v>
@@ -2271,7 +2269,7 @@
         <v>0</v>
       </c>
       <c r="T11">
-        <v>2473</v>
+        <v>2506</v>
       </c>
       <c r="U11">
         <v>5222</v>
@@ -2330,7 +2328,7 @@
         <v>44166</v>
       </c>
       <c r="N12">
-        <v>259316</v>
+        <v>259697</v>
       </c>
       <c r="O12">
         <v>559871</v>
@@ -2348,7 +2346,7 @@
         <v>0</v>
       </c>
       <c r="T12">
-        <v>1136</v>
+        <v>1035</v>
       </c>
       <c r="U12">
         <v>3394</v>
@@ -2362,7 +2360,7 @@
       <c r="X12">
         <v>1619461</v>
       </c>
-      <c r="Y12" s="2" t="s">
+      <c r="Y12" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2407,7 +2405,7 @@
         <v>44165</v>
       </c>
       <c r="N13">
-        <v>258180</v>
+        <v>258662</v>
       </c>
       <c r="O13">
         <v>556477</v>
@@ -2425,7 +2423,7 @@
         <v>0</v>
       </c>
       <c r="T13">
-        <v>803</v>
+        <v>823</v>
       </c>
       <c r="U13">
         <v>2429</v>
@@ -2484,7 +2482,7 @@
         <v>44164</v>
       </c>
       <c r="N14">
-        <v>257377</v>
+        <v>257839</v>
       </c>
       <c r="O14">
         <v>554048</v>
@@ -2502,7 +2500,7 @@
         <v>0</v>
       </c>
       <c r="T14">
-        <v>1245</v>
+        <v>1251</v>
       </c>
       <c r="U14">
         <v>3404</v>
@@ -2561,7 +2559,7 @@
         <v>44163</v>
       </c>
       <c r="N15">
-        <v>256132</v>
+        <v>256588</v>
       </c>
       <c r="O15">
         <v>550644</v>
@@ -2579,7 +2577,7 @@
         <v>0</v>
       </c>
       <c r="T15">
-        <v>1372</v>
+        <v>1392</v>
       </c>
       <c r="U15">
         <v>3499</v>
@@ -2638,7 +2636,7 @@
         <v>44162</v>
       </c>
       <c r="N16">
-        <v>254760</v>
+        <v>255196</v>
       </c>
       <c r="O16">
         <v>547145</v>
@@ -2656,7 +2654,7 @@
         <v>0</v>
       </c>
       <c r="T16">
-        <v>1336</v>
+        <v>1387</v>
       </c>
       <c r="U16">
         <v>2247</v>
@@ -2715,7 +2713,7 @@
         <v>44161</v>
       </c>
       <c r="N17">
-        <v>253424</v>
+        <v>253809</v>
       </c>
       <c r="O17">
         <v>544898</v>
@@ -2733,7 +2731,7 @@
         <v>0</v>
       </c>
       <c r="T17">
-        <v>2289</v>
+        <v>2280</v>
       </c>
       <c r="U17">
         <v>4568</v>
@@ -2792,7 +2790,7 @@
         <v>44160</v>
       </c>
       <c r="N18">
-        <v>251135</v>
+        <v>251529</v>
       </c>
       <c r="O18">
         <v>540330</v>
@@ -2810,7 +2808,7 @@
         <v>0</v>
       </c>
       <c r="T18">
-        <v>2066</v>
+        <v>2106</v>
       </c>
       <c r="U18">
         <v>4591</v>
@@ -2869,7 +2867,7 @@
         <v>44159</v>
       </c>
       <c r="N19">
-        <v>249069</v>
+        <v>249423</v>
       </c>
       <c r="O19">
         <v>535739</v>
@@ -2887,7 +2885,7 @@
         <v>0</v>
       </c>
       <c r="T19">
-        <v>955</v>
+        <v>858</v>
       </c>
       <c r="U19">
         <v>2985</v>
@@ -2946,7 +2944,7 @@
         <v>44158</v>
       </c>
       <c r="N20">
-        <v>248114</v>
+        <v>248565</v>
       </c>
       <c r="O20">
         <v>532754</v>
@@ -2964,7 +2962,7 @@
         <v>0</v>
       </c>
       <c r="T20">
-        <v>898</v>
+        <v>917</v>
       </c>
       <c r="U20">
         <v>2291</v>
@@ -3023,7 +3021,7 @@
         <v>44157</v>
       </c>
       <c r="N21">
-        <v>247216</v>
+        <v>247648</v>
       </c>
       <c r="O21">
         <v>530463</v>
@@ -3041,7 +3039,7 @@
         <v>0</v>
       </c>
       <c r="T21">
-        <v>1512</v>
+        <v>1554</v>
       </c>
       <c r="U21">
         <v>3340</v>
@@ -3100,7 +3098,7 @@
         <v>44156</v>
       </c>
       <c r="N22">
-        <v>245704</v>
+        <v>246094</v>
       </c>
       <c r="O22">
         <v>527123</v>
@@ -3118,7 +3116,7 @@
         <v>0</v>
       </c>
       <c r="T22">
-        <v>1884</v>
+        <v>1894</v>
       </c>
       <c r="U22">
         <v>3891</v>
@@ -3177,7 +3175,7 @@
         <v>44155</v>
       </c>
       <c r="N23">
-        <v>243820</v>
+        <v>244200</v>
       </c>
       <c r="O23">
         <v>523232</v>
@@ -3195,7 +3193,7 @@
         <v>0</v>
       </c>
       <c r="T23">
-        <v>1967</v>
+        <v>2020</v>
       </c>
       <c r="U23">
         <v>4420</v>
@@ -3254,7 +3252,7 @@
         <v>44154</v>
       </c>
       <c r="N24">
-        <v>241853</v>
+        <v>242180</v>
       </c>
       <c r="O24">
         <v>518812</v>
@@ -3272,7 +3270,7 @@
         <v>0</v>
       </c>
       <c r="T24">
-        <v>1864</v>
+        <v>1882</v>
       </c>
       <c r="U24">
         <v>4384</v>
@@ -3331,7 +3329,7 @@
         <v>44153</v>
       </c>
       <c r="N25">
-        <v>239989</v>
+        <v>240298</v>
       </c>
       <c r="O25">
         <v>514428</v>
@@ -3349,7 +3347,7 @@
         <v>0</v>
       </c>
       <c r="T25">
-        <v>1555</v>
+        <v>1562</v>
       </c>
       <c r="U25">
         <v>3812</v>
@@ -3408,7 +3406,7 @@
         <v>44152</v>
       </c>
       <c r="N26">
-        <v>238434</v>
+        <v>238736</v>
       </c>
       <c r="O26">
         <v>510616</v>
@@ -3426,7 +3424,7 @@
         <v>0</v>
       </c>
       <c r="T26">
-        <v>619</v>
+        <v>609</v>
       </c>
       <c r="U26">
         <v>3033</v>
@@ -3485,7 +3483,7 @@
         <v>44151</v>
       </c>
       <c r="N27">
-        <v>237815</v>
+        <v>238127</v>
       </c>
       <c r="O27">
         <v>507583</v>
@@ -3503,7 +3501,7 @@
         <v>0</v>
       </c>
       <c r="T27">
-        <v>687</v>
+        <v>708</v>
       </c>
       <c r="U27">
         <v>1868</v>
@@ -3562,7 +3560,7 @@
         <v>44150</v>
       </c>
       <c r="N28">
-        <v>237128</v>
+        <v>237419</v>
       </c>
       <c r="O28">
         <v>505715</v>
@@ -3580,7 +3578,7 @@
         <v>0</v>
       </c>
       <c r="T28">
-        <v>1331</v>
+        <v>1352</v>
       </c>
       <c r="U28">
         <v>3424</v>
@@ -3639,7 +3637,7 @@
         <v>44149</v>
       </c>
       <c r="N29">
-        <v>235797</v>
+        <v>236067</v>
       </c>
       <c r="O29">
         <v>502291</v>
@@ -3657,7 +3655,7 @@
         <v>0</v>
       </c>
       <c r="T29">
-        <v>1268</v>
+        <v>1304</v>
       </c>
       <c r="U29">
         <v>3686</v>
@@ -3716,7 +3714,7 @@
         <v>44148</v>
       </c>
       <c r="N30">
-        <v>234529</v>
+        <v>234763</v>
       </c>
       <c r="O30">
         <v>498605</v>
@@ -3734,7 +3732,7 @@
         <v>0</v>
       </c>
       <c r="T30">
-        <v>1119</v>
+        <v>1111</v>
       </c>
       <c r="U30">
         <v>3551</v>
@@ -3793,7 +3791,7 @@
         <v>44147</v>
       </c>
       <c r="N31">
-        <v>233410</v>
+        <v>233652</v>
       </c>
       <c r="O31">
         <v>495054</v>
@@ -3811,7 +3809,7 @@
         <v>0</v>
       </c>
       <c r="T31">
-        <v>1563</v>
+        <v>1579</v>
       </c>
       <c r="U31">
         <v>3275</v>
@@ -3870,7 +3868,7 @@
         <v>44146</v>
       </c>
       <c r="N32">
-        <v>231847</v>
+        <v>232073</v>
       </c>
       <c r="O32">
         <v>491779</v>
@@ -3888,7 +3886,7 @@
         <v>0</v>
       </c>
       <c r="T32">
-        <v>1360</v>
+        <v>1357</v>
       </c>
       <c r="U32">
         <v>4033</v>
@@ -3947,7 +3945,7 @@
         <v>44145</v>
       </c>
       <c r="N33">
-        <v>230487</v>
+        <v>230716</v>
       </c>
       <c r="O33">
         <v>487746</v>
@@ -3965,7 +3963,7 @@
         <v>0</v>
       </c>
       <c r="T33">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="U33">
         <v>2261</v>
@@ -4024,7 +4022,7 @@
         <v>44144</v>
       </c>
       <c r="N34">
-        <v>229910</v>
+        <v>230136</v>
       </c>
       <c r="O34">
         <v>485485</v>
@@ -4042,7 +4040,7 @@
         <v>0</v>
       </c>
       <c r="T34">
-        <v>496</v>
+        <v>501</v>
       </c>
       <c r="U34">
         <v>1467</v>
@@ -4101,7 +4099,7 @@
         <v>44143</v>
       </c>
       <c r="N35">
-        <v>229414</v>
+        <v>229635</v>
       </c>
       <c r="O35">
         <v>484018</v>
@@ -4119,7 +4117,7 @@
         <v>0</v>
       </c>
       <c r="T35">
-        <v>1119</v>
+        <v>1132</v>
       </c>
       <c r="U35">
         <v>2297</v>
@@ -4178,7 +4176,7 @@
         <v>44142</v>
       </c>
       <c r="N36">
-        <v>228295</v>
+        <v>228503</v>
       </c>
       <c r="O36">
         <v>481721</v>
@@ -4196,7 +4194,7 @@
         <v>0</v>
       </c>
       <c r="T36">
-        <v>1173</v>
+        <v>1186</v>
       </c>
       <c r="U36">
         <v>3143</v>
@@ -4255,7 +4253,7 @@
         <v>44141</v>
       </c>
       <c r="N37">
-        <v>227122</v>
+        <v>227317</v>
       </c>
       <c r="O37">
         <v>478578</v>
@@ -4273,7 +4271,7 @@
         <v>0</v>
       </c>
       <c r="T37">
-        <v>1146</v>
+        <v>1155</v>
       </c>
       <c r="U37">
         <v>2541</v>
@@ -4332,7 +4330,7 @@
         <v>44140</v>
       </c>
       <c r="N38">
-        <v>225976</v>
+        <v>226162</v>
       </c>
       <c r="O38">
         <v>476037</v>
@@ -4350,7 +4348,7 @@
         <v>0</v>
       </c>
       <c r="T38">
-        <v>1117</v>
+        <v>1126</v>
       </c>
       <c r="U38">
         <v>3114</v>
@@ -4409,7 +4407,7 @@
         <v>44139</v>
       </c>
       <c r="N39">
-        <v>224859</v>
+        <v>225036</v>
       </c>
       <c r="O39">
         <v>472923</v>
@@ -4427,7 +4425,7 @@
         <v>0</v>
       </c>
       <c r="T39">
-        <v>1514</v>
+        <v>1525</v>
       </c>
       <c r="U39">
         <v>3115</v>
@@ -4486,7 +4484,7 @@
         <v>44138</v>
       </c>
       <c r="N40">
-        <v>223345</v>
+        <v>223511</v>
       </c>
       <c r="O40">
         <v>469808</v>
@@ -4504,7 +4502,7 @@
         <v>0</v>
       </c>
       <c r="T40">
-        <v>491</v>
+        <v>474</v>
       </c>
       <c r="U40">
         <v>1446</v>
@@ -4518,7 +4516,7 @@
       <c r="X40">
         <v>1336795</v>
       </c>
-      <c r="Y40" s="2" t="s">
+      <c r="Y40" t="s">
         <v>63</v>
       </c>
     </row>
@@ -4563,7 +4561,7 @@
         <v>44137</v>
       </c>
       <c r="N41">
-        <v>222854</v>
+        <v>223037</v>
       </c>
       <c r="O41">
         <v>468362</v>
@@ -4581,7 +4579,7 @@
         <v>0</v>
       </c>
       <c r="T41">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="U41">
         <v>1166</v>
@@ -4640,7 +4638,7 @@
         <v>44136</v>
       </c>
       <c r="N42">
-        <v>222459</v>
+        <v>222639</v>
       </c>
       <c r="O42">
         <v>467196</v>
@@ -4658,7 +4656,7 @@
         <v>0</v>
       </c>
       <c r="T42">
-        <v>963</v>
+        <v>970</v>
       </c>
       <c r="U42">
         <v>2082</v>
@@ -4717,7 +4715,7 @@
         <v>44135</v>
       </c>
       <c r="N43">
-        <v>221496</v>
+        <v>221669</v>
       </c>
       <c r="O43">
         <v>465114</v>
@@ -4794,7 +4792,7 @@
         <v>44134</v>
       </c>
       <c r="N44">
-        <v>220549</v>
+        <v>220722</v>
       </c>
       <c r="O44">
         <v>462713</v>
@@ -4812,7 +4810,7 @@
         <v>0</v>
       </c>
       <c r="T44">
-        <v>1037</v>
+        <v>1055</v>
       </c>
       <c r="U44">
         <v>2334</v>
@@ -4871,7 +4869,7 @@
         <v>44133</v>
       </c>
       <c r="N45">
-        <v>219512</v>
+        <v>219667</v>
       </c>
       <c r="O45">
         <v>460379</v>
@@ -4889,7 +4887,7 @@
         <v>0</v>
       </c>
       <c r="T45">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="U45">
         <v>2464</v>
@@ -4948,7 +4946,7 @@
         <v>44132</v>
       </c>
       <c r="N46">
-        <v>218468</v>
+        <v>218622</v>
       </c>
       <c r="O46">
         <v>457915</v>
@@ -4966,7 +4964,7 @@
         <v>0</v>
       </c>
       <c r="T46">
-        <v>919</v>
+        <v>929</v>
       </c>
       <c r="U46">
         <v>2253</v>
@@ -4980,7 +4978,7 @@
       <c r="X46">
         <v>1097470</v>
       </c>
-      <c r="Y46" t="s">
+      <c r="Y46" s="2" t="s">
         <v>69</v>
       </c>
     </row>
@@ -5025,7 +5023,7 @@
         <v>44131</v>
       </c>
       <c r="N47">
-        <v>217549</v>
+        <v>217693</v>
       </c>
       <c r="O47">
         <v>455662</v>
@@ -5043,7 +5041,7 @@
         <v>0</v>
       </c>
       <c r="T47">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="U47">
         <v>1754</v>
@@ -5102,7 +5100,7 @@
         <v>44130</v>
       </c>
       <c r="N48">
-        <v>217147</v>
+        <v>217294</v>
       </c>
       <c r="O48">
         <v>453908</v>
@@ -5120,7 +5118,7 @@
         <v>0</v>
       </c>
       <c r="T48">
-        <v>382</v>
+        <v>387</v>
       </c>
       <c r="U48">
         <v>1076</v>
@@ -5179,7 +5177,7 @@
         <v>44129</v>
       </c>
       <c r="N49">
-        <v>216765</v>
+        <v>216907</v>
       </c>
       <c r="O49">
         <v>452832</v>
@@ -5197,7 +5195,7 @@
         <v>0</v>
       </c>
       <c r="T49">
-        <v>890</v>
+        <v>897</v>
       </c>
       <c r="U49">
         <v>1793</v>
@@ -5256,7 +5254,7 @@
         <v>44128</v>
       </c>
       <c r="N50">
-        <v>215875</v>
+        <v>216010</v>
       </c>
       <c r="O50">
         <v>451039</v>
@@ -5274,7 +5272,7 @@
         <v>0</v>
       </c>
       <c r="T50">
-        <v>934</v>
+        <v>941</v>
       </c>
       <c r="U50">
         <v>15071</v>
@@ -5333,7 +5331,7 @@
         <v>44127</v>
       </c>
       <c r="N51">
-        <v>214941</v>
+        <v>215069</v>
       </c>
       <c r="O51">
         <v>435968</v>
@@ -5410,7 +5408,7 @@
         <v>44126</v>
       </c>
       <c r="N52">
-        <v>213815</v>
+        <v>213943</v>
       </c>
       <c r="O52">
         <v>433472</v>
@@ -5428,7 +5426,7 @@
         <v>0</v>
       </c>
       <c r="T52">
-        <v>1019</v>
+        <v>1025</v>
       </c>
       <c r="U52">
         <v>2131</v>
@@ -5487,7 +5485,7 @@
         <v>44125</v>
       </c>
       <c r="N53">
-        <v>212796</v>
+        <v>212918</v>
       </c>
       <c r="O53">
         <v>431341</v>
@@ -5505,7 +5503,7 @@
         <v>0</v>
       </c>
       <c r="T53">
-        <v>837</v>
+        <v>830</v>
       </c>
       <c r="U53">
         <v>2265</v>
@@ -5564,7 +5562,7 @@
         <v>44124</v>
       </c>
       <c r="N54">
-        <v>211959</v>
+        <v>212088</v>
       </c>
       <c r="O54">
         <v>429076</v>
@@ -5582,7 +5580,7 @@
         <v>0</v>
       </c>
       <c r="T54">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="U54">
         <v>1666</v>
@@ -5641,7 +5639,7 @@
         <v>44123</v>
       </c>
       <c r="N55">
-        <v>211503</v>
+        <v>211637</v>
       </c>
       <c r="O55">
         <v>427410</v>
@@ -5718,7 +5716,7 @@
         <v>44122</v>
       </c>
       <c r="N56">
-        <v>211101</v>
+        <v>211235</v>
       </c>
       <c r="O56">
         <v>426597</v>
@@ -5736,7 +5734,7 @@
         <v>0</v>
       </c>
       <c r="T56">
-        <v>773</v>
+        <v>777</v>
       </c>
       <c r="U56">
         <v>1528</v>
@@ -5795,7 +5793,7 @@
         <v>44121</v>
       </c>
       <c r="N57">
-        <v>210328</v>
+        <v>210458</v>
       </c>
       <c r="O57">
         <v>425069</v>
@@ -5813,7 +5811,7 @@
         <v>0</v>
       </c>
       <c r="T57">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="U57">
         <v>1864</v>
@@ -5872,7 +5870,7 @@
         <v>44120</v>
       </c>
       <c r="N58">
-        <v>209431</v>
+        <v>209564</v>
       </c>
       <c r="O58">
         <v>423205</v>
@@ -5890,7 +5888,7 @@
         <v>0</v>
       </c>
       <c r="T58">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="U58">
         <v>1999</v>
@@ -5949,7 +5947,7 @@
         <v>44119</v>
       </c>
       <c r="N59">
-        <v>208501</v>
+        <v>208636</v>
       </c>
       <c r="O59">
         <v>421206</v>
@@ -5967,7 +5965,7 @@
         <v>0</v>
       </c>
       <c r="T59">
-        <v>807</v>
+        <v>798</v>
       </c>
       <c r="U59">
         <v>2455</v>
@@ -6026,7 +6024,7 @@
         <v>44118</v>
       </c>
       <c r="N60">
-        <v>207694</v>
+        <v>207838</v>
       </c>
       <c r="O60">
         <v>418751</v>
@@ -6044,7 +6042,7 @@
         <v>0</v>
       </c>
       <c r="T60">
-        <v>698</v>
+        <v>724</v>
       </c>
       <c r="U60">
         <v>2008</v>
@@ -6103,7 +6101,7 @@
         <v>44117</v>
       </c>
       <c r="N61">
-        <v>206996</v>
+        <v>207114</v>
       </c>
       <c r="O61">
         <v>416743</v>
@@ -6121,7 +6119,7 @@
         <v>0</v>
       </c>
       <c r="T61">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="U61">
         <v>1169</v>
@@ -6180,7 +6178,7 @@
         <v>44116</v>
       </c>
       <c r="N62">
-        <v>206714</v>
+        <v>206829</v>
       </c>
       <c r="O62">
         <v>415574</v>
@@ -6198,7 +6196,7 @@
         <v>0</v>
       </c>
       <c r="T62">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="U62">
         <v>981</v>
@@ -6257,7 +6255,7 @@
         <v>44115</v>
       </c>
       <c r="N63">
-        <v>206246</v>
+        <v>206360</v>
       </c>
       <c r="O63">
         <v>414593</v>
@@ -6275,7 +6273,7 @@
         <v>0</v>
       </c>
       <c r="T63">
-        <v>681</v>
+        <v>690</v>
       </c>
       <c r="U63">
         <v>1472</v>
@@ -6334,7 +6332,7 @@
         <v>44114</v>
       </c>
       <c r="N64">
-        <v>205565</v>
+        <v>205670</v>
       </c>
       <c r="O64">
         <v>413121</v>
@@ -6352,7 +6350,7 @@
         <v>0</v>
       </c>
       <c r="T64">
-        <v>898</v>
+        <v>905</v>
       </c>
       <c r="U64">
         <v>1727</v>
@@ -6411,7 +6409,7 @@
         <v>44113</v>
       </c>
       <c r="N65">
-        <v>204667</v>
+        <v>204765</v>
       </c>
       <c r="O65">
         <v>411394</v>
@@ -6429,7 +6427,7 @@
         <v>0</v>
       </c>
       <c r="T65">
-        <v>985</v>
+        <v>988</v>
       </c>
       <c r="U65">
         <v>2131</v>
@@ -6488,7 +6486,7 @@
         <v>44112</v>
       </c>
       <c r="N66">
-        <v>203682</v>
+        <v>203777</v>
       </c>
       <c r="O66">
         <v>409263</v>
@@ -6506,7 +6504,7 @@
         <v>0</v>
       </c>
       <c r="T66">
-        <v>925</v>
+        <v>922</v>
       </c>
       <c r="U66">
         <v>2140</v>
@@ -6565,7 +6563,7 @@
         <v>44111</v>
       </c>
       <c r="N67">
-        <v>202757</v>
+        <v>202855</v>
       </c>
       <c r="O67">
         <v>407123</v>
@@ -6583,7 +6581,7 @@
         <v>0</v>
       </c>
       <c r="T67">
-        <v>610</v>
+        <v>622</v>
       </c>
       <c r="U67">
         <v>-768</v>
@@ -6642,7 +6640,7 @@
         <v>44110</v>
       </c>
       <c r="N68">
-        <v>202147</v>
+        <v>202233</v>
       </c>
       <c r="O68">
         <v>407891</v>
@@ -6660,7 +6658,7 @@
         <v>0</v>
       </c>
       <c r="T68">
-        <v>344</v>
+        <v>330</v>
       </c>
       <c r="U68">
         <v>1486</v>
@@ -6719,7 +6717,7 @@
         <v>44109</v>
       </c>
       <c r="N69">
-        <v>201803</v>
+        <v>201903</v>
       </c>
       <c r="O69">
         <v>406405</v>
@@ -6737,7 +6735,7 @@
         <v>0</v>
       </c>
       <c r="T69">
-        <v>365</v>
+        <v>373</v>
       </c>
       <c r="U69">
         <v>663</v>
@@ -6796,7 +6794,7 @@
         <v>44108</v>
       </c>
       <c r="N70">
-        <v>201438</v>
+        <v>201530</v>
       </c>
       <c r="O70">
         <v>405742</v>
@@ -6814,7 +6812,7 @@
         <v>0</v>
       </c>
       <c r="T70">
-        <v>740</v>
+        <v>743</v>
       </c>
       <c r="U70">
         <v>1083</v>
@@ -6873,7 +6871,7 @@
         <v>44107</v>
       </c>
       <c r="N71">
-        <v>200698</v>
+        <v>200787</v>
       </c>
       <c r="O71">
         <v>404659</v>
@@ -6891,7 +6889,7 @@
         <v>0</v>
       </c>
       <c r="T71">
-        <v>847</v>
+        <v>844</v>
       </c>
       <c r="U71">
         <v>1433</v>
@@ -6950,7 +6948,7 @@
         <v>44106</v>
       </c>
       <c r="N72">
-        <v>199851</v>
+        <v>199943</v>
       </c>
       <c r="O72">
         <v>403226</v>
@@ -6968,7 +6966,7 @@
         <v>0</v>
       </c>
       <c r="T72">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="U72">
         <v>1732</v>
@@ -7027,7 +7025,7 @@
         <v>44105</v>
       </c>
       <c r="N73">
-        <v>198993</v>
+        <v>199084</v>
       </c>
       <c r="O73">
         <v>401494</v>
@@ -7045,7 +7043,7 @@
         <v>0</v>
       </c>
       <c r="T73">
-        <v>1063</v>
+        <v>1060</v>
       </c>
       <c r="U73">
         <v>1638</v>
@@ -7104,7 +7102,7 @@
         <v>44104</v>
       </c>
       <c r="N74">
-        <v>197930</v>
+        <v>198024</v>
       </c>
       <c r="O74">
         <v>399856</v>
@@ -7122,7 +7120,7 @@
         <v>0</v>
       </c>
       <c r="T74">
-        <v>737</v>
+        <v>732</v>
       </c>
       <c r="U74">
         <v>1651</v>
@@ -7181,7 +7179,7 @@
         <v>44103</v>
       </c>
       <c r="N75">
-        <v>197193</v>
+        <v>197292</v>
       </c>
       <c r="O75">
         <v>398205</v>
@@ -7199,7 +7197,7 @@
         <v>0</v>
       </c>
       <c r="T75">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="U75">
         <v>1223</v>
@@ -7258,7 +7256,7 @@
         <v>44102</v>
       </c>
       <c r="N76">
-        <v>196946</v>
+        <v>197047</v>
       </c>
       <c r="O76">
         <v>396982</v>
@@ -7276,7 +7274,7 @@
         <v>0</v>
       </c>
       <c r="T76">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="U76">
         <v>613</v>
@@ -7290,7 +7288,7 @@
       <c r="X76">
         <v>906676</v>
       </c>
-      <c r="Y76" t="s">
+      <c r="Y76" s="2" t="s">
         <v>99</v>
       </c>
     </row>
@@ -7335,7 +7333,7 @@
         <v>44101</v>
       </c>
       <c r="N77">
-        <v>196640</v>
+        <v>196740</v>
       </c>
       <c r="O77">
         <v>396369</v>
@@ -7353,7 +7351,7 @@
         <v>0</v>
       </c>
       <c r="T77">
-        <v>871</v>
+        <v>874</v>
       </c>
       <c r="U77">
         <v>1197</v>
@@ -7412,7 +7410,7 @@
         <v>44100</v>
       </c>
       <c r="N78">
-        <v>195769</v>
+        <v>195866</v>
       </c>
       <c r="O78">
         <v>395172</v>
@@ -7430,7 +7428,7 @@
         <v>0</v>
       </c>
       <c r="T78">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="U78">
         <v>1320</v>
@@ -7489,7 +7487,7 @@
         <v>44099</v>
       </c>
       <c r="N79">
-        <v>194919</v>
+        <v>195017</v>
       </c>
       <c r="O79">
         <v>393852</v>
@@ -7507,7 +7505,7 @@
         <v>0</v>
       </c>
       <c r="T79">
-        <v>939</v>
+        <v>933</v>
       </c>
       <c r="U79">
         <v>1495</v>
@@ -7566,7 +7564,7 @@
         <v>44098</v>
       </c>
       <c r="N80">
-        <v>193980</v>
+        <v>194084</v>
       </c>
       <c r="O80">
         <v>392357</v>
@@ -7584,7 +7582,7 @@
         <v>0</v>
       </c>
       <c r="T80">
-        <v>1154</v>
+        <v>1159</v>
       </c>
       <c r="U80">
         <v>1449</v>
@@ -7643,7 +7641,7 @@
         <v>44097</v>
       </c>
       <c r="N81">
-        <v>192826</v>
+        <v>192925</v>
       </c>
       <c r="O81">
         <v>390908</v>
@@ -7661,7 +7659,7 @@
         <v>0</v>
       </c>
       <c r="T81">
-        <v>864</v>
+        <v>859</v>
       </c>
       <c r="U81">
         <v>1519</v>
@@ -7720,7 +7718,7 @@
         <v>44096</v>
       </c>
       <c r="N82">
-        <v>191962</v>
+        <v>192066</v>
       </c>
       <c r="O82">
         <v>389389</v>
@@ -7738,7 +7736,7 @@
         <v>0</v>
       </c>
       <c r="T82">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="U82">
         <v>1103</v>
@@ -7797,7 +7795,7 @@
         <v>44095</v>
       </c>
       <c r="N83">
-        <v>191682</v>
+        <v>191783</v>
       </c>
       <c r="O83">
         <v>388286</v>
@@ -7815,7 +7813,7 @@
         <v>0</v>
       </c>
       <c r="T83">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="U83">
         <v>525</v>
@@ -7874,7 +7872,7 @@
         <v>44094</v>
       </c>
       <c r="N84">
-        <v>191359</v>
+        <v>191459</v>
       </c>
       <c r="O84">
         <v>387761</v>
@@ -7892,7 +7890,7 @@
         <v>0</v>
       </c>
       <c r="T84">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="U84">
         <v>1036</v>
@@ -7951,7 +7949,7 @@
         <v>44093</v>
       </c>
       <c r="N85">
-        <v>190612</v>
+        <v>190708</v>
       </c>
       <c r="O85">
         <v>386725</v>
@@ -7969,7 +7967,7 @@
         <v>0</v>
       </c>
       <c r="T85">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="U85">
         <v>1416</v>
@@ -8028,7 +8026,7 @@
         <v>44092</v>
       </c>
       <c r="N86">
-        <v>189712</v>
+        <v>189807</v>
       </c>
       <c r="O86">
         <v>385309</v>
@@ -8046,7 +8044,7 @@
         <v>0</v>
       </c>
       <c r="T86">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="U86">
         <v>1544</v>
@@ -8105,7 +8103,7 @@
         <v>44091</v>
       </c>
       <c r="N87">
-        <v>188832</v>
+        <v>188929</v>
       </c>
       <c r="O87">
         <v>383765</v>
@@ -8123,7 +8121,7 @@
         <v>0</v>
       </c>
       <c r="T87">
-        <v>1178</v>
+        <v>1184</v>
       </c>
       <c r="U87">
         <v>1475</v>
@@ -8182,7 +8180,7 @@
         <v>44090</v>
       </c>
       <c r="N88">
-        <v>187654</v>
+        <v>187745</v>
       </c>
       <c r="O88">
         <v>382290</v>
@@ -8200,7 +8198,7 @@
         <v>0</v>
       </c>
       <c r="T88">
-        <v>1045</v>
+        <v>1040</v>
       </c>
       <c r="U88">
         <v>1453</v>
@@ -8259,7 +8257,7 @@
         <v>44089</v>
       </c>
       <c r="N89">
-        <v>186609</v>
+        <v>186705</v>
       </c>
       <c r="O89">
         <v>380837</v>
@@ -8277,7 +8275,7 @@
         <v>0</v>
       </c>
       <c r="T89">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="U89">
         <v>956</v>
@@ -8336,7 +8334,7 @@
         <v>44088</v>
       </c>
       <c r="N90">
-        <v>186201</v>
+        <v>186300</v>
       </c>
       <c r="O90">
         <v>379881</v>
@@ -8413,7 +8411,7 @@
         <v>44087</v>
       </c>
       <c r="N91">
-        <v>185811</v>
+        <v>185910</v>
       </c>
       <c r="O91">
         <v>379336</v>
@@ -8431,7 +8429,7 @@
         <v>0</v>
       </c>
       <c r="T91">
-        <v>818</v>
+        <v>821</v>
       </c>
       <c r="U91">
         <v>1132</v>
@@ -8490,7 +8488,7 @@
         <v>44086</v>
       </c>
       <c r="N92">
-        <v>184993</v>
+        <v>185089</v>
       </c>
       <c r="O92">
         <v>378204</v>
@@ -8508,7 +8506,7 @@
         <v>0</v>
       </c>
       <c r="T92">
-        <v>1008</v>
+        <v>1014</v>
       </c>
       <c r="U92">
         <v>1516</v>
@@ -8567,7 +8565,7 @@
         <v>44085</v>
       </c>
       <c r="N93">
-        <v>183985</v>
+        <v>184075</v>
       </c>
       <c r="O93">
         <v>376688</v>
@@ -8585,7 +8583,7 @@
         <v>0</v>
       </c>
       <c r="T93">
-        <v>1161</v>
+        <v>1156</v>
       </c>
       <c r="U93">
         <v>1496</v>
@@ -8644,7 +8642,7 @@
         <v>44084</v>
       </c>
       <c r="N94">
-        <v>182824</v>
+        <v>182919</v>
       </c>
       <c r="O94">
         <v>375192</v>
@@ -8662,7 +8660,7 @@
         <v>0</v>
       </c>
       <c r="T94">
-        <v>1102</v>
+        <v>1092</v>
       </c>
       <c r="U94">
         <v>1934</v>
@@ -8721,7 +8719,7 @@
         <v>44083</v>
       </c>
       <c r="N95">
-        <v>181722</v>
+        <v>181827</v>
       </c>
       <c r="O95">
         <v>373258</v>
@@ -8739,7 +8737,7 @@
         <v>0</v>
       </c>
       <c r="T95">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="U95">
         <v>979</v>
@@ -8798,7 +8796,7 @@
         <v>44082</v>
       </c>
       <c r="N96">
-        <v>181370</v>
+        <v>181477</v>
       </c>
       <c r="O96">
         <v>372279</v>
@@ -8816,7 +8814,7 @@
         <v>0</v>
       </c>
       <c r="T96">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="U96">
         <v>474</v>
@@ -8875,7 +8873,7 @@
         <v>44081</v>
       </c>
       <c r="N97">
-        <v>181144</v>
+        <v>181250</v>
       </c>
       <c r="O97">
         <v>371805</v>
@@ -8893,7 +8891,7 @@
         <v>0</v>
       </c>
       <c r="T97">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="U97">
         <v>499</v>
@@ -8952,7 +8950,7 @@
         <v>44080</v>
       </c>
       <c r="N98">
-        <v>180697</v>
+        <v>180802</v>
       </c>
       <c r="O98">
         <v>371306</v>
@@ -8970,7 +8968,7 @@
         <v>0</v>
       </c>
       <c r="T98">
-        <v>921</v>
+        <v>926</v>
       </c>
       <c r="U98">
         <v>1187</v>
@@ -9029,7 +9027,7 @@
         <v>44079</v>
       </c>
       <c r="N99">
-        <v>179776</v>
+        <v>179876</v>
       </c>
       <c r="O99">
         <v>370119</v>
@@ -9047,7 +9045,7 @@
         <v>0</v>
       </c>
       <c r="T99">
-        <v>996</v>
+        <v>1002</v>
       </c>
       <c r="U99">
         <v>1227</v>
@@ -9106,7 +9104,7 @@
         <v>44078</v>
       </c>
       <c r="N100">
-        <v>178780</v>
+        <v>178874</v>
       </c>
       <c r="O100">
         <v>368892</v>
@@ -9124,7 +9122,7 @@
         <v>0</v>
       </c>
       <c r="T100">
-        <v>1076</v>
+        <v>1071</v>
       </c>
       <c r="U100">
         <v>1491</v>
@@ -9183,7 +9181,7 @@
         <v>44077</v>
       </c>
       <c r="N101">
-        <v>177704</v>
+        <v>177803</v>
       </c>
       <c r="O101">
         <v>367401</v>
@@ -9201,7 +9199,7 @@
         <v>0</v>
       </c>
       <c r="T101">
-        <v>1026</v>
+        <v>1032</v>
       </c>
       <c r="U101">
         <v>1513</v>
@@ -9260,7 +9258,7 @@
         <v>44076</v>
       </c>
       <c r="N102">
-        <v>176678</v>
+        <v>176771</v>
       </c>
       <c r="O102">
         <v>365888</v>
@@ -9278,7 +9276,7 @@
         <v>0</v>
       </c>
       <c r="T102">
-        <v>1022</v>
+        <v>1019</v>
       </c>
       <c r="U102">
         <v>1839</v>
@@ -9337,7 +9335,7 @@
         <v>44075</v>
       </c>
       <c r="N103">
-        <v>175656</v>
+        <v>175752</v>
       </c>
       <c r="O103">
         <v>364049</v>
@@ -9355,7 +9353,7 @@
         <v>0</v>
       </c>
       <c r="T103">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="U103">
         <v>751</v>
@@ -9414,7 +9412,7 @@
         <v>44074</v>
       </c>
       <c r="N104">
-        <v>175274</v>
+        <v>175375</v>
       </c>
       <c r="O104">
         <v>363298</v>
@@ -9491,7 +9489,7 @@
         <v>44073</v>
       </c>
       <c r="N105">
-        <v>174800</v>
+        <v>174901</v>
       </c>
       <c r="O105">
         <v>362636</v>
@@ -9509,7 +9507,7 @@
         <v>0</v>
       </c>
       <c r="T105">
-        <v>1008</v>
+        <v>1015</v>
       </c>
       <c r="U105">
         <v>1284</v>
@@ -9568,7 +9566,7 @@
         <v>44072</v>
       </c>
       <c r="N106">
-        <v>173792</v>
+        <v>173886</v>
       </c>
       <c r="O106">
         <v>361352</v>
@@ -9586,7 +9584,7 @@
         <v>0</v>
       </c>
       <c r="T106">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="U106">
         <v>1627</v>
@@ -9645,7 +9643,7 @@
         <v>44071</v>
       </c>
       <c r="N107">
-        <v>172766</v>
+        <v>172862</v>
       </c>
       <c r="O107">
         <v>359725</v>
@@ -9663,7 +9661,7 @@
         <v>0</v>
       </c>
       <c r="T107">
-        <v>1124</v>
+        <v>1128</v>
       </c>
       <c r="U107">
         <v>1659</v>
@@ -9722,7 +9720,7 @@
         <v>44070</v>
       </c>
       <c r="N108">
-        <v>171642</v>
+        <v>171734</v>
       </c>
       <c r="O108">
         <v>358066</v>
@@ -9740,7 +9738,7 @@
         <v>0</v>
       </c>
       <c r="T108">
-        <v>1305</v>
+        <v>1297</v>
       </c>
       <c r="U108">
         <v>1819</v>
@@ -9799,7 +9797,7 @@
         <v>44069</v>
       </c>
       <c r="N109">
-        <v>170337</v>
+        <v>170437</v>
       </c>
       <c r="O109">
         <v>356247</v>
@@ -9817,7 +9815,7 @@
         <v>0</v>
       </c>
       <c r="T109">
-        <v>1140</v>
+        <v>1145</v>
       </c>
       <c r="U109">
         <v>1954</v>
@@ -9876,7 +9874,7 @@
         <v>44068</v>
       </c>
       <c r="N110">
-        <v>169197</v>
+        <v>169292</v>
       </c>
       <c r="O110">
         <v>354293</v>
@@ -9894,7 +9892,7 @@
         <v>0</v>
       </c>
       <c r="T110">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="U110">
         <v>1075</v>
@@ -9953,7 +9951,7 @@
         <v>44067</v>
       </c>
       <c r="N111">
-        <v>168845</v>
+        <v>168948</v>
       </c>
       <c r="O111">
         <v>353218</v>
@@ -10030,7 +10028,7 @@
         <v>44066</v>
       </c>
       <c r="N112">
-        <v>168271</v>
+        <v>168374</v>
       </c>
       <c r="O112">
         <v>352520</v>
@@ -10048,7 +10046,7 @@
         <v>0</v>
       </c>
       <c r="T112">
-        <v>1028</v>
+        <v>1036</v>
       </c>
       <c r="U112">
         <v>1598</v>
@@ -10107,7 +10105,7 @@
         <v>44065</v>
       </c>
       <c r="N113">
-        <v>167243</v>
+        <v>167338</v>
       </c>
       <c r="O113">
         <v>350922</v>
@@ -10125,7 +10123,7 @@
         <v>0</v>
       </c>
       <c r="T113">
-        <v>1110</v>
+        <v>1117</v>
       </c>
       <c r="U113">
         <v>1767</v>
@@ -10184,7 +10182,7 @@
         <v>44064</v>
       </c>
       <c r="N114">
-        <v>166133</v>
+        <v>166221</v>
       </c>
       <c r="O114">
         <v>349155</v>
@@ -10202,7 +10200,7 @@
         <v>0</v>
       </c>
       <c r="T114">
-        <v>1134</v>
+        <v>1122</v>
       </c>
       <c r="U114">
         <v>1975</v>
@@ -10261,7 +10259,7 @@
         <v>44063</v>
       </c>
       <c r="N115">
-        <v>164999</v>
+        <v>165099</v>
       </c>
       <c r="O115">
         <v>347180</v>
@@ -10279,7 +10277,7 @@
         <v>0</v>
       </c>
       <c r="T115">
-        <v>1424</v>
+        <v>1413</v>
       </c>
       <c r="U115">
         <v>1996</v>
@@ -10338,7 +10336,7 @@
         <v>44062</v>
       </c>
       <c r="N116">
-        <v>163575</v>
+        <v>163686</v>
       </c>
       <c r="O116">
         <v>345184</v>
@@ -10356,7 +10354,7 @@
         <v>0</v>
       </c>
       <c r="T116">
-        <v>1195</v>
+        <v>1188</v>
       </c>
       <c r="U116">
         <v>2227</v>
@@ -10415,7 +10413,7 @@
         <v>44061</v>
       </c>
       <c r="N117">
-        <v>162380</v>
+        <v>162498</v>
       </c>
       <c r="O117">
         <v>342957</v>
@@ -10433,7 +10431,7 @@
         <v>0</v>
       </c>
       <c r="T117">
-        <v>419</v>
+        <v>409</v>
       </c>
       <c r="U117">
         <v>1274</v>
@@ -10492,7 +10490,7 @@
         <v>44060</v>
       </c>
       <c r="N118">
-        <v>161961</v>
+        <v>162089</v>
       </c>
       <c r="O118">
         <v>341683</v>
@@ -10569,7 +10567,7 @@
         <v>44059</v>
       </c>
       <c r="N119">
-        <v>161343</v>
+        <v>161471</v>
       </c>
       <c r="O119">
         <v>340998</v>
@@ -10587,7 +10585,7 @@
         <v>0</v>
       </c>
       <c r="T119">
-        <v>1218</v>
+        <v>1226</v>
       </c>
       <c r="U119">
         <v>1881</v>
@@ -10646,7 +10644,7 @@
         <v>44058</v>
       </c>
       <c r="N120">
-        <v>160125</v>
+        <v>160245</v>
       </c>
       <c r="O120">
         <v>339117</v>
@@ -10664,7 +10662,7 @@
         <v>0</v>
       </c>
       <c r="T120">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="U120">
         <v>2143</v>
@@ -10723,7 +10721,7 @@
         <v>44057</v>
       </c>
       <c r="N121">
-        <v>158906</v>
+        <v>159025</v>
       </c>
       <c r="O121">
         <v>336974</v>
@@ -10800,7 +10798,7 @@
         <v>44056</v>
       </c>
       <c r="N122">
-        <v>157742</v>
+        <v>157861</v>
       </c>
       <c r="O122">
         <v>334323</v>
@@ -10818,7 +10816,7 @@
         <v>0</v>
       </c>
       <c r="T122">
-        <v>1518</v>
+        <v>1513</v>
       </c>
       <c r="U122">
         <v>2988</v>
@@ -10877,7 +10875,7 @@
         <v>44055</v>
       </c>
       <c r="N123">
-        <v>156224</v>
+        <v>156348</v>
       </c>
       <c r="O123">
         <v>331335</v>
@@ -10895,7 +10893,7 @@
         <v>0</v>
       </c>
       <c r="T123">
-        <v>1323</v>
+        <v>1330</v>
       </c>
       <c r="U123">
         <v>2599</v>
@@ -10954,7 +10952,7 @@
         <v>44054</v>
       </c>
       <c r="N124">
-        <v>154901</v>
+        <v>155018</v>
       </c>
       <c r="O124">
         <v>328736</v>
@@ -10972,7 +10970,7 @@
         <v>0</v>
       </c>
       <c r="T124">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="U124">
         <v>1594</v>
@@ -11031,7 +11029,7 @@
         <v>44053</v>
       </c>
       <c r="N125">
-        <v>154466</v>
+        <v>154588</v>
       </c>
       <c r="O125">
         <v>327142</v>
@@ -11049,7 +11047,7 @@
         <v>0</v>
       </c>
       <c r="T125">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="U125">
         <v>862</v>
@@ -11108,7 +11106,7 @@
         <v>44052</v>
       </c>
       <c r="N126">
-        <v>153852</v>
+        <v>153973</v>
       </c>
       <c r="O126">
         <v>326280</v>
@@ -11185,7 +11183,7 @@
         <v>44051</v>
       </c>
       <c r="N127">
-        <v>152768</v>
+        <v>152889</v>
       </c>
       <c r="O127">
         <v>324801</v>
@@ -11203,7 +11201,7 @@
         <v>0</v>
       </c>
       <c r="T127">
-        <v>1333</v>
+        <v>1331</v>
       </c>
       <c r="U127">
         <v>7992</v>
@@ -11262,7 +11260,7 @@
         <v>44050</v>
       </c>
       <c r="N128">
-        <v>151435</v>
+        <v>151558</v>
       </c>
       <c r="O128">
         <v>316809</v>
@@ -11280,7 +11278,7 @@
         <v>0</v>
       </c>
       <c r="T128">
-        <v>1248</v>
+        <v>1237</v>
       </c>
       <c r="U128">
         <v>2594</v>
@@ -11339,7 +11337,7 @@
         <v>44049</v>
       </c>
       <c r="N129">
-        <v>150187</v>
+        <v>150321</v>
       </c>
       <c r="O129">
         <v>314215</v>
@@ -11357,7 +11355,7 @@
         <v>0</v>
       </c>
       <c r="T129">
-        <v>1360</v>
+        <v>1355</v>
       </c>
       <c r="U129">
         <v>2123</v>
@@ -11416,7 +11414,7 @@
         <v>44048</v>
       </c>
       <c r="N130">
-        <v>148827</v>
+        <v>148966</v>
       </c>
       <c r="O130">
         <v>312092</v>
@@ -11434,7 +11432,7 @@
         <v>0</v>
       </c>
       <c r="T130">
-        <v>1239</v>
+        <v>1244</v>
       </c>
       <c r="U130">
         <v>4408</v>
@@ -11493,7 +11491,7 @@
         <v>44047</v>
       </c>
       <c r="N131">
-        <v>147588</v>
+        <v>147722</v>
       </c>
       <c r="O131">
         <v>307684</v>
@@ -11511,7 +11509,7 @@
         <v>0</v>
       </c>
       <c r="T131">
-        <v>536</v>
+        <v>517</v>
       </c>
       <c r="U131">
         <v>1606</v>
@@ -11570,7 +11568,7 @@
         <v>44046</v>
       </c>
       <c r="N132">
-        <v>147052</v>
+        <v>147205</v>
       </c>
       <c r="O132">
         <v>306078</v>
@@ -11647,7 +11645,7 @@
         <v>44045</v>
       </c>
       <c r="N133">
-        <v>146558</v>
+        <v>146711</v>
       </c>
       <c r="O133">
         <v>305247</v>
@@ -11665,7 +11663,7 @@
         <v>0</v>
       </c>
       <c r="T133">
-        <v>1192</v>
+        <v>1198</v>
       </c>
       <c r="U133">
         <v>2366</v>
@@ -11724,7 +11722,7 @@
         <v>44044</v>
       </c>
       <c r="N134">
-        <v>145366</v>
+        <v>145513</v>
       </c>
       <c r="O134">
         <v>302881</v>
@@ -11742,7 +11740,7 @@
         <v>0</v>
       </c>
       <c r="T134">
-        <v>1313</v>
+        <v>1329</v>
       </c>
       <c r="U134">
         <v>2533</v>
@@ -11756,7 +11754,7 @@
       <c r="X134">
         <v>994993</v>
       </c>
-      <c r="Y134" s="2" t="s">
+      <c r="Y134" t="s">
         <v>157</v>
       </c>
     </row>
@@ -11801,7 +11799,7 @@
         <v>44043</v>
       </c>
       <c r="N135">
-        <v>144053</v>
+        <v>144184</v>
       </c>
       <c r="O135">
         <v>300348</v>
@@ -11819,7 +11817,7 @@
         <v>0</v>
       </c>
       <c r="T135">
-        <v>1248</v>
+        <v>1245</v>
       </c>
       <c r="U135">
         <v>3279</v>
@@ -11878,7 +11876,7 @@
         <v>44042</v>
       </c>
       <c r="N136">
-        <v>142805</v>
+        <v>142939</v>
       </c>
       <c r="O136">
         <v>297069</v>
@@ -11896,7 +11894,7 @@
         <v>0</v>
       </c>
       <c r="T136">
-        <v>1491</v>
+        <v>1497</v>
       </c>
       <c r="U136">
         <v>2868</v>
@@ -11955,7 +11953,7 @@
         <v>44041</v>
       </c>
       <c r="N137">
-        <v>141314</v>
+        <v>141442</v>
       </c>
       <c r="O137">
         <v>294201</v>
@@ -11973,7 +11971,7 @@
         <v>0</v>
       </c>
       <c r="T137">
-        <v>1128</v>
+        <v>1125</v>
       </c>
       <c r="U137">
         <v>4051</v>
@@ -12032,7 +12030,7 @@
         <v>44040</v>
       </c>
       <c r="N138">
-        <v>140186</v>
+        <v>140317</v>
       </c>
       <c r="O138">
         <v>290150</v>
@@ -12050,7 +12048,7 @@
         <v>0</v>
       </c>
       <c r="T138">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="U138">
         <v>1671</v>
@@ -12109,7 +12107,7 @@
         <v>44039</v>
       </c>
       <c r="N139">
-        <v>139121</v>
+        <v>139254</v>
       </c>
       <c r="O139">
         <v>288479</v>
@@ -12186,7 +12184,7 @@
         <v>44038</v>
       </c>
       <c r="N140">
-        <v>138561</v>
+        <v>138694</v>
       </c>
       <c r="O140">
         <v>287099</v>
@@ -12204,7 +12202,7 @@
         <v>0</v>
       </c>
       <c r="T140">
-        <v>1005</v>
+        <v>1009</v>
       </c>
       <c r="U140">
         <v>1811</v>
@@ -12263,7 +12261,7 @@
         <v>44037</v>
       </c>
       <c r="N141">
-        <v>137556</v>
+        <v>137685</v>
       </c>
       <c r="O141">
         <v>285288</v>
@@ -12281,7 +12279,7 @@
         <v>0</v>
       </c>
       <c r="T141">
-        <v>1192</v>
+        <v>1180</v>
       </c>
       <c r="U141">
         <v>3040</v>
@@ -12340,7 +12338,7 @@
         <v>44036</v>
       </c>
       <c r="N142">
-        <v>136364</v>
+        <v>136505</v>
       </c>
       <c r="O142">
         <v>282248</v>
@@ -12358,7 +12356,7 @@
         <v>0</v>
       </c>
       <c r="T142">
-        <v>1061</v>
+        <v>1074</v>
       </c>
       <c r="U142">
         <v>2378</v>
@@ -12417,7 +12415,7 @@
         <v>44035</v>
       </c>
       <c r="N143">
-        <v>135303</v>
+        <v>135431</v>
       </c>
       <c r="O143">
         <v>279870</v>
@@ -12435,7 +12433,7 @@
         <v>0</v>
       </c>
       <c r="T143">
-        <v>1134</v>
+        <v>1142</v>
       </c>
       <c r="U143">
         <v>2246</v>
@@ -12494,7 +12492,7 @@
         <v>44034</v>
       </c>
       <c r="N144">
-        <v>134169</v>
+        <v>134289</v>
       </c>
       <c r="O144">
         <v>277624</v>
@@ -12512,7 +12510,7 @@
         <v>0</v>
       </c>
       <c r="T144">
-        <v>1069</v>
+        <v>1046</v>
       </c>
       <c r="U144">
         <v>2510</v>
@@ -12571,7 +12569,7 @@
         <v>44033</v>
       </c>
       <c r="N145">
-        <v>133100</v>
+        <v>133243</v>
       </c>
       <c r="O145">
         <v>275114</v>
@@ -12589,7 +12587,7 @@
         <v>0</v>
       </c>
       <c r="T145">
-        <v>369</v>
+        <v>375</v>
       </c>
       <c r="U145">
         <v>1623</v>
@@ -12648,7 +12646,7 @@
         <v>44032</v>
       </c>
       <c r="N146">
-        <v>132731</v>
+        <v>132868</v>
       </c>
       <c r="O146">
         <v>273491</v>
@@ -12725,7 +12723,7 @@
         <v>44031</v>
       </c>
       <c r="N147">
-        <v>132204</v>
+        <v>132341</v>
       </c>
       <c r="O147">
         <v>272603</v>
@@ -12743,7 +12741,7 @@
         <v>0</v>
       </c>
       <c r="T147">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="U147">
         <v>1976</v>
@@ -12802,7 +12800,7 @@
         <v>44030</v>
       </c>
       <c r="N148">
-        <v>131331</v>
+        <v>131467</v>
       </c>
       <c r="O148">
         <v>270627</v>
@@ -12820,7 +12818,7 @@
         <v>0</v>
       </c>
       <c r="T148">
-        <v>936</v>
+        <v>942</v>
       </c>
       <c r="U148">
         <v>2480</v>
@@ -12879,7 +12877,7 @@
         <v>44029</v>
       </c>
       <c r="N149">
-        <v>130395</v>
+        <v>130525</v>
       </c>
       <c r="O149">
         <v>268147</v>
@@ -12897,7 +12895,7 @@
         <v>0</v>
       </c>
       <c r="T149">
-        <v>953</v>
+        <v>940</v>
       </c>
       <c r="U149">
         <v>2195</v>
@@ -12956,7 +12954,7 @@
         <v>44028</v>
       </c>
       <c r="N150">
-        <v>129442</v>
+        <v>129585</v>
       </c>
       <c r="O150">
         <v>265952</v>
@@ -12974,7 +12972,7 @@
         <v>0</v>
       </c>
       <c r="T150">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="U150">
         <v>2404</v>
@@ -13033,7 +13031,7 @@
         <v>44027</v>
       </c>
       <c r="N151">
-        <v>128582</v>
+        <v>128726</v>
       </c>
       <c r="O151">
         <v>263548</v>
@@ -13051,7 +13049,7 @@
         <v>0</v>
       </c>
       <c r="T151">
-        <v>739</v>
+        <v>745</v>
       </c>
       <c r="U151">
         <v>2212</v>
@@ -13110,7 +13108,7 @@
         <v>44026</v>
       </c>
       <c r="N152">
-        <v>127843</v>
+        <v>127981</v>
       </c>
       <c r="O152">
         <v>261336</v>
@@ -13128,7 +13126,7 @@
         <v>0</v>
       </c>
       <c r="T152">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="U152">
         <v>1174</v>
@@ -13187,7 +13185,7 @@
         <v>44025</v>
       </c>
       <c r="N153">
-        <v>127512</v>
+        <v>127651</v>
       </c>
       <c r="O153">
         <v>260162</v>
@@ -13264,7 +13262,7 @@
         <v>44024</v>
       </c>
       <c r="N154">
-        <v>127038</v>
+        <v>127177</v>
       </c>
       <c r="O154">
         <v>259268</v>
@@ -13282,7 +13280,7 @@
         <v>0</v>
       </c>
       <c r="T154">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="U154">
         <v>5070</v>
@@ -13341,7 +13339,7 @@
         <v>44023</v>
       </c>
       <c r="N155">
-        <v>126286</v>
+        <v>126424</v>
       </c>
       <c r="O155">
         <v>254198</v>
@@ -13359,7 +13357,7 @@
         <v>0</v>
       </c>
       <c r="T155">
-        <v>822</v>
+        <v>835</v>
       </c>
       <c r="U155">
         <v>2207</v>
@@ -13418,7 +13416,7 @@
         <v>44022</v>
       </c>
       <c r="N156">
-        <v>125464</v>
+        <v>125589</v>
       </c>
       <c r="O156">
         <v>251991</v>
@@ -13436,7 +13434,7 @@
         <v>0</v>
       </c>
       <c r="T156">
-        <v>900</v>
+        <v>865</v>
       </c>
       <c r="U156">
         <v>1654</v>
@@ -13495,7 +13493,7 @@
         <v>44021</v>
       </c>
       <c r="N157">
-        <v>124564</v>
+        <v>124724</v>
       </c>
       <c r="O157">
         <v>250337</v>
@@ -13513,7 +13511,7 @@
         <v>0</v>
       </c>
       <c r="T157">
-        <v>812</v>
+        <v>818</v>
       </c>
       <c r="U157">
         <v>1888</v>
@@ -13572,7 +13570,7 @@
         <v>44020</v>
       </c>
       <c r="N158">
-        <v>123752</v>
+        <v>123906</v>
       </c>
       <c r="O158">
         <v>248449</v>
@@ -13590,7 +13588,7 @@
         <v>0</v>
       </c>
       <c r="T158">
-        <v>905</v>
+        <v>910</v>
       </c>
       <c r="U158">
         <v>1936</v>
@@ -13649,7 +13647,7 @@
         <v>44019</v>
       </c>
       <c r="N159">
-        <v>122847</v>
+        <v>122996</v>
       </c>
       <c r="O159">
         <v>246513</v>
@@ -13667,7 +13665,7 @@
         <v>0</v>
       </c>
       <c r="T159">
-        <v>266</v>
+        <v>235</v>
       </c>
       <c r="U159">
         <v>818</v>
@@ -13726,7 +13724,7 @@
         <v>44018</v>
       </c>
       <c r="N160">
-        <v>122581</v>
+        <v>122761</v>
       </c>
       <c r="O160">
         <v>245695</v>
@@ -13803,7 +13801,7 @@
         <v>44017</v>
       </c>
       <c r="N161">
-        <v>122374</v>
+        <v>122554</v>
       </c>
       <c r="O161">
         <v>245113</v>
@@ -13880,7 +13878,7 @@
         <v>44016</v>
       </c>
       <c r="N162">
-        <v>122074</v>
+        <v>122254</v>
       </c>
       <c r="O162">
         <v>244241</v>
@@ -13957,7 +13955,7 @@
         <v>44015</v>
       </c>
       <c r="N163">
-        <v>121472</v>
+        <v>121652</v>
       </c>
       <c r="O163">
         <v>242897</v>
@@ -13975,7 +13973,7 @@
         <v>0</v>
       </c>
       <c r="T163">
-        <v>696</v>
+        <v>699</v>
       </c>
       <c r="U163">
         <v>1694</v>
@@ -14034,7 +14032,7 @@
         <v>44014</v>
       </c>
       <c r="N164">
-        <v>120776</v>
+        <v>120953</v>
       </c>
       <c r="O164">
         <v>241203</v>
@@ -14052,7 +14050,7 @@
         <v>0</v>
       </c>
       <c r="T164">
-        <v>689</v>
+        <v>696</v>
       </c>
       <c r="U164">
         <v>1433</v>
@@ -14111,7 +14109,7 @@
         <v>44013</v>
       </c>
       <c r="N165">
-        <v>120087</v>
+        <v>120257</v>
       </c>
       <c r="O165">
         <v>239770</v>
@@ -14129,7 +14127,7 @@
         <v>0</v>
       </c>
       <c r="T165">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="U165">
         <v>1483</v>
@@ -14188,7 +14186,7 @@
         <v>44012</v>
       </c>
       <c r="N166">
-        <v>119503</v>
+        <v>119677</v>
       </c>
       <c r="O166">
         <v>238287</v>
@@ -14206,7 +14204,7 @@
         <v>0</v>
       </c>
       <c r="T166">
-        <v>358</v>
+        <v>338</v>
       </c>
       <c r="U166">
         <v>734</v>
@@ -14265,7 +14263,7 @@
         <v>44011</v>
       </c>
       <c r="N167">
-        <v>119145</v>
+        <v>119339</v>
       </c>
       <c r="O167">
         <v>237553</v>
@@ -14283,7 +14281,7 @@
         <v>0</v>
       </c>
       <c r="T167">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="U167">
         <v>547</v>
@@ -14342,7 +14340,7 @@
         <v>44010</v>
       </c>
       <c r="N168">
-        <v>118874</v>
+        <v>119066</v>
       </c>
       <c r="O168">
         <v>237006</v>
@@ -14360,7 +14358,7 @@
         <v>0</v>
       </c>
       <c r="T168">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="U168">
         <v>1048</v>
@@ -14419,7 +14417,7 @@
         <v>44009</v>
       </c>
       <c r="N169">
-        <v>118372</v>
+        <v>118563</v>
       </c>
       <c r="O169">
         <v>235958</v>
@@ -14437,7 +14435,7 @@
         <v>0</v>
       </c>
       <c r="T169">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="U169">
         <v>1546</v>
@@ -14496,7 +14494,7 @@
         <v>44008</v>
       </c>
       <c r="N170">
-        <v>117748</v>
+        <v>117942</v>
       </c>
       <c r="O170">
         <v>234412</v>
@@ -14514,7 +14512,7 @@
         <v>0</v>
       </c>
       <c r="T170">
-        <v>663</v>
+        <v>647</v>
       </c>
       <c r="U170">
         <v>1279</v>
@@ -14573,7 +14571,7 @@
         <v>44007</v>
       </c>
       <c r="N171">
-        <v>117085</v>
+        <v>117295</v>
       </c>
       <c r="O171">
         <v>233133</v>
@@ -14650,7 +14648,7 @@
         <v>44006</v>
       </c>
       <c r="N172">
-        <v>116378</v>
+        <v>116588</v>
       </c>
       <c r="O172">
         <v>231878</v>
@@ -14668,7 +14666,7 @@
         <v>0</v>
       </c>
       <c r="T172">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="U172">
         <v>1262</v>
@@ -14727,7 +14725,7 @@
         <v>44005</v>
       </c>
       <c r="N173">
-        <v>115653</v>
+        <v>115866</v>
       </c>
       <c r="O173">
         <v>230616</v>
@@ -14745,7 +14743,7 @@
         <v>0</v>
       </c>
       <c r="T173">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="U173">
         <v>847</v>
@@ -14804,7 +14802,7 @@
         <v>44004</v>
       </c>
       <c r="N174">
-        <v>115359</v>
+        <v>115577</v>
       </c>
       <c r="O174">
         <v>229769</v>
@@ -14836,7 +14834,7 @@
       <c r="X174">
         <v>528099</v>
       </c>
-      <c r="Y174" s="2" t="s">
+      <c r="Y174" t="s">
         <v>197</v>
       </c>
     </row>
@@ -14881,7 +14879,7 @@
         <v>44003</v>
       </c>
       <c r="N175">
-        <v>115066</v>
+        <v>115284</v>
       </c>
       <c r="O175">
         <v>229250</v>
@@ -14899,7 +14897,7 @@
         <v>0</v>
       </c>
       <c r="T175">
-        <v>611</v>
+        <v>615</v>
       </c>
       <c r="U175">
         <v>686</v>
@@ -14958,7 +14956,7 @@
         <v>44002</v>
       </c>
       <c r="N176">
-        <v>114455</v>
+        <v>114669</v>
       </c>
       <c r="O176">
         <v>228564</v>
@@ -14976,7 +14974,7 @@
         <v>0</v>
       </c>
       <c r="T176">
-        <v>656</v>
+        <v>649</v>
       </c>
       <c r="U176">
         <v>1587</v>
@@ -15035,7 +15033,7 @@
         <v>44001</v>
       </c>
       <c r="N177">
-        <v>113799</v>
+        <v>114020</v>
       </c>
       <c r="O177">
         <v>226977</v>
@@ -15053,7 +15051,7 @@
         <v>0</v>
       </c>
       <c r="T177">
-        <v>693</v>
+        <v>685</v>
       </c>
       <c r="U177">
         <v>1095</v>
@@ -15112,7 +15110,7 @@
         <v>44000</v>
       </c>
       <c r="N178">
-        <v>113106</v>
+        <v>113335</v>
       </c>
       <c r="O178">
         <v>225882</v>
@@ -15130,7 +15128,7 @@
         <v>0</v>
       </c>
       <c r="T178">
-        <v>794</v>
+        <v>779</v>
       </c>
       <c r="U178">
         <v>1081</v>
@@ -15189,7 +15187,7 @@
         <v>43999</v>
       </c>
       <c r="N179">
-        <v>112312</v>
+        <v>112556</v>
       </c>
       <c r="O179">
         <v>224801</v>
@@ -15207,7 +15205,7 @@
         <v>0</v>
       </c>
       <c r="T179">
-        <v>706</v>
+        <v>718</v>
       </c>
       <c r="U179">
         <v>1173</v>
@@ -15266,7 +15264,7 @@
         <v>43998</v>
       </c>
       <c r="N180">
-        <v>111606</v>
+        <v>111838</v>
       </c>
       <c r="O180">
         <v>223628</v>
@@ -15284,7 +15282,7 @@
         <v>0</v>
       </c>
       <c r="T180">
-        <v>406</v>
+        <v>387</v>
       </c>
       <c r="U180">
         <v>688</v>
@@ -15343,7 +15341,7 @@
         <v>43997</v>
       </c>
       <c r="N181">
-        <v>111200</v>
+        <v>111451</v>
       </c>
       <c r="O181">
         <v>222940</v>
@@ -15361,7 +15359,7 @@
         <v>0</v>
       </c>
       <c r="T181">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="U181">
         <v>610</v>
@@ -15420,7 +15418,7 @@
         <v>43996</v>
       </c>
       <c r="N182">
-        <v>110845</v>
+        <v>111095</v>
       </c>
       <c r="O182">
         <v>222330</v>
@@ -15438,7 +15436,7 @@
         <v>0</v>
       </c>
       <c r="T182">
-        <v>690</v>
+        <v>693</v>
       </c>
       <c r="U182">
         <v>943</v>
@@ -15497,7 +15495,7 @@
         <v>43995</v>
       </c>
       <c r="N183">
-        <v>110155</v>
+        <v>110402</v>
       </c>
       <c r="O183">
         <v>221387</v>
@@ -15515,7 +15513,7 @@
         <v>0</v>
       </c>
       <c r="T183">
-        <v>763</v>
+        <v>766</v>
       </c>
       <c r="U183">
         <v>1380</v>
@@ -15574,7 +15572,7 @@
         <v>43994</v>
       </c>
       <c r="N184">
-        <v>109392</v>
+        <v>109636</v>
       </c>
       <c r="O184">
         <v>220007</v>
@@ -15592,7 +15590,7 @@
         <v>0</v>
       </c>
       <c r="T184">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="U184">
         <v>1527</v>
@@ -15651,7 +15649,7 @@
         <v>43993</v>
       </c>
       <c r="N185">
-        <v>108493</v>
+        <v>108738</v>
       </c>
       <c r="O185">
         <v>218480</v>
@@ -15669,7 +15667,7 @@
         <v>0</v>
       </c>
       <c r="T185">
-        <v>884</v>
+        <v>888</v>
       </c>
       <c r="U185">
         <v>1237</v>
@@ -15728,7 +15726,7 @@
         <v>43992</v>
       </c>
       <c r="N186">
-        <v>107609</v>
+        <v>107850</v>
       </c>
       <c r="O186">
         <v>217243</v>
@@ -15746,7 +15744,7 @@
         <v>0</v>
       </c>
       <c r="T186">
-        <v>901</v>
+        <v>891</v>
       </c>
       <c r="U186">
         <v>1263</v>
@@ -15805,7 +15803,7 @@
         <v>43991</v>
       </c>
       <c r="N187">
-        <v>106708</v>
+        <v>106959</v>
       </c>
       <c r="O187">
         <v>215980</v>
@@ -15823,7 +15821,7 @@
         <v>0</v>
       </c>
       <c r="T187">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="U187">
         <v>1095</v>
@@ -15882,7 +15880,7 @@
         <v>43990</v>
       </c>
       <c r="N188">
-        <v>106032</v>
+        <v>106285</v>
       </c>
       <c r="O188">
         <v>214885</v>
@@ -15959,7 +15957,7 @@
         <v>43989</v>
       </c>
       <c r="N189">
-        <v>105586</v>
+        <v>105839</v>
       </c>
       <c r="O189">
         <v>214230</v>
@@ -15977,7 +15975,7 @@
         <v>0</v>
       </c>
       <c r="T189">
-        <v>711</v>
+        <v>714</v>
       </c>
       <c r="U189">
         <v>982</v>
@@ -16036,7 +16034,7 @@
         <v>43988</v>
       </c>
       <c r="N190">
-        <v>104875</v>
+        <v>105125</v>
       </c>
       <c r="O190">
         <v>213248</v>
@@ -16054,7 +16052,7 @@
         <v>0</v>
       </c>
       <c r="T190">
-        <v>844</v>
+        <v>837</v>
       </c>
       <c r="U190">
         <v>1513</v>
@@ -16113,7 +16111,7 @@
         <v>43987</v>
       </c>
       <c r="N191">
-        <v>104031</v>
+        <v>104288</v>
       </c>
       <c r="O191">
         <v>211735</v>
@@ -16131,7 +16129,7 @@
         <v>0</v>
       </c>
       <c r="T191">
-        <v>864</v>
+        <v>881</v>
       </c>
       <c r="U191">
         <v>-2849</v>
@@ -16190,7 +16188,7 @@
         <v>43986</v>
       </c>
       <c r="N192">
-        <v>103167</v>
+        <v>103407</v>
       </c>
       <c r="O192">
         <v>214584</v>
@@ -16208,7 +16206,7 @@
         <v>0</v>
       </c>
       <c r="T192">
-        <v>980</v>
+        <v>974</v>
       </c>
       <c r="U192">
         <v>2145</v>
@@ -16267,7 +16265,7 @@
         <v>43985</v>
       </c>
       <c r="N193">
-        <v>102187</v>
+        <v>102433</v>
       </c>
       <c r="O193">
         <v>212439</v>
@@ -16285,7 +16283,7 @@
         <v>0</v>
       </c>
       <c r="T193">
-        <v>1000</v>
+        <v>973</v>
       </c>
       <c r="U193">
         <v>1736</v>
@@ -16344,7 +16342,7 @@
         <v>43984</v>
       </c>
       <c r="N194">
-        <v>101187</v>
+        <v>101460</v>
       </c>
       <c r="O194">
         <v>210703</v>
@@ -16362,7 +16360,7 @@
         <v>0</v>
       </c>
       <c r="T194">
-        <v>671</v>
+        <v>680</v>
       </c>
       <c r="U194">
         <v>2858</v>
@@ -16421,7 +16419,7 @@
         <v>43983</v>
       </c>
       <c r="N195">
-        <v>100516</v>
+        <v>100780</v>
       </c>
       <c r="O195">
         <v>207845</v>
@@ -16439,7 +16437,7 @@
         <v>0</v>
       </c>
       <c r="T195">
-        <v>651</v>
+        <v>653</v>
       </c>
       <c r="U195">
         <v>896</v>
@@ -16498,7 +16496,7 @@
         <v>43982</v>
       </c>
       <c r="N196">
-        <v>99865</v>
+        <v>100127</v>
       </c>
       <c r="O196">
         <v>206949</v>
@@ -16516,7 +16514,7 @@
         <v>0</v>
       </c>
       <c r="T196">
-        <v>918</v>
+        <v>925</v>
       </c>
       <c r="U196">
         <v>1425</v>
@@ -16530,7 +16528,7 @@
       <c r="X196">
         <v>447976</v>
       </c>
-      <c r="Y196" t="s">
+      <c r="Y196" s="2" t="s">
         <v>219</v>
       </c>
     </row>
@@ -16575,7 +16573,7 @@
         <v>43981</v>
       </c>
       <c r="N197">
-        <v>98947</v>
+        <v>99202</v>
       </c>
       <c r="O197">
         <v>205524</v>
@@ -16593,7 +16591,7 @@
         <v>0</v>
       </c>
       <c r="T197">
-        <v>1169</v>
+        <v>1171</v>
       </c>
       <c r="U197">
         <v>1565</v>
@@ -16652,7 +16650,7 @@
         <v>43980</v>
       </c>
       <c r="N198">
-        <v>97778</v>
+        <v>98031</v>
       </c>
       <c r="O198">
         <v>203959</v>
@@ -16670,7 +16668,7 @@
         <v>0</v>
       </c>
       <c r="T198">
-        <v>1242</v>
+        <v>1238</v>
       </c>
       <c r="U198">
         <v>1596</v>
@@ -16729,7 +16727,7 @@
         <v>43979</v>
       </c>
       <c r="N199">
-        <v>96536</v>
+        <v>96793</v>
       </c>
       <c r="O199">
         <v>202363</v>
@@ -16747,7 +16745,7 @@
         <v>0</v>
       </c>
       <c r="T199">
-        <v>1316</v>
+        <v>1335</v>
       </c>
       <c r="U199">
         <v>1563</v>
@@ -16806,7 +16804,7 @@
         <v>43978</v>
       </c>
       <c r="N200">
-        <v>95220</v>
+        <v>95458</v>
       </c>
       <c r="O200">
         <v>200800</v>
@@ -16824,7 +16822,7 @@
         <v>0</v>
       </c>
       <c r="T200">
-        <v>672</v>
+        <v>665</v>
       </c>
       <c r="U200">
         <v>17287</v>
@@ -16883,7 +16881,7 @@
         <v>43977</v>
       </c>
       <c r="N201">
-        <v>94548</v>
+        <v>94793</v>
       </c>
       <c r="O201">
         <v>183513</v>
@@ -16901,7 +16899,7 @@
         <v>0</v>
       </c>
       <c r="T201">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="U201">
         <v>901</v>
@@ -16960,7 +16958,7 @@
         <v>43976</v>
       </c>
       <c r="N202">
-        <v>93994</v>
+        <v>94238</v>
       </c>
       <c r="O202">
         <v>182612</v>
@@ -16978,7 +16976,7 @@
         <v>0</v>
       </c>
       <c r="T202">
-        <v>684</v>
+        <v>689</v>
       </c>
       <c r="U202">
         <v>1027</v>
@@ -17037,7 +17035,7 @@
         <v>43975</v>
       </c>
       <c r="N203">
-        <v>93310</v>
+        <v>93549</v>
       </c>
       <c r="O203">
         <v>181585</v>
@@ -17055,7 +17053,7 @@
         <v>0</v>
       </c>
       <c r="T203">
-        <v>1035</v>
+        <v>1038</v>
       </c>
       <c r="U203">
         <v>1383</v>
@@ -17114,7 +17112,7 @@
         <v>43974</v>
       </c>
       <c r="N204">
-        <v>92275</v>
+        <v>92511</v>
       </c>
       <c r="O204">
         <v>180202</v>
@@ -17132,7 +17130,7 @@
         <v>0</v>
       </c>
       <c r="T204">
-        <v>1303</v>
+        <v>1291</v>
       </c>
       <c r="U204">
         <v>3945</v>
@@ -17191,7 +17189,7 @@
         <v>43973</v>
       </c>
       <c r="N205">
-        <v>90972</v>
+        <v>91220</v>
       </c>
       <c r="O205">
         <v>176257</v>
@@ -17209,7 +17207,7 @@
         <v>0</v>
       </c>
       <c r="T205">
-        <v>1427</v>
+        <v>1377</v>
       </c>
       <c r="U205">
         <v>4547</v>
@@ -17223,7 +17221,7 @@
       <c r="X205">
         <v>497331</v>
       </c>
-      <c r="Y205" t="s">
+      <c r="Y205" s="2" t="s">
         <v>228</v>
       </c>
     </row>
@@ -17268,7 +17266,7 @@
         <v>43972</v>
       </c>
       <c r="N206">
-        <v>89545</v>
+        <v>89843</v>
       </c>
       <c r="O206">
         <v>171710</v>
@@ -17286,7 +17284,7 @@
         <v>0</v>
       </c>
       <c r="T206">
-        <v>1390</v>
+        <v>1399</v>
       </c>
       <c r="U206">
         <v>1759</v>
@@ -17345,7 +17343,7 @@
         <v>43971</v>
       </c>
       <c r="N207">
-        <v>88155</v>
+        <v>88444</v>
       </c>
       <c r="O207">
         <v>169951</v>
@@ -17363,7 +17361,7 @@
         <v>0</v>
       </c>
       <c r="T207">
-        <v>1332</v>
+        <v>1318</v>
       </c>
       <c r="U207">
         <v>1549</v>
@@ -17422,7 +17420,7 @@
         <v>43970</v>
       </c>
       <c r="N208">
-        <v>86823</v>
+        <v>87126</v>
       </c>
       <c r="O208">
         <v>168402</v>
@@ -17440,7 +17438,7 @@
         <v>0</v>
       </c>
       <c r="T208">
-        <v>889</v>
+        <v>855</v>
       </c>
       <c r="U208">
         <v>1133</v>
@@ -17499,7 +17497,7 @@
         <v>43969</v>
       </c>
       <c r="N209">
-        <v>85934</v>
+        <v>86271</v>
       </c>
       <c r="O209">
         <v>167269</v>
@@ -17517,7 +17515,7 @@
         <v>0</v>
       </c>
       <c r="T209">
-        <v>850</v>
+        <v>873</v>
       </c>
       <c r="U209">
         <v>1130</v>
@@ -17576,7 +17574,7 @@
         <v>43968</v>
       </c>
       <c r="N210">
-        <v>85084</v>
+        <v>85398</v>
       </c>
       <c r="O210">
         <v>166139</v>
@@ -17594,7 +17592,7 @@
         <v>0</v>
       </c>
       <c r="T210">
-        <v>1195</v>
+        <v>1237</v>
       </c>
       <c r="U210">
         <v>1798</v>
@@ -17653,7 +17651,7 @@
         <v>43967</v>
       </c>
       <c r="N211">
-        <v>83889</v>
+        <v>84161</v>
       </c>
       <c r="O211">
         <v>164341</v>
@@ -17671,7 +17669,7 @@
         <v>0</v>
       </c>
       <c r="T211">
-        <v>1263</v>
+        <v>1535</v>
       </c>
       <c r="U211">
         <v>1313</v>

</xml_diff>